<commit_message>
pop up modal changes
</commit_message>
<xml_diff>
--- a/data/leaguedata.xlsx
+++ b/data/leaguedata.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -34,6 +34,9 @@
     <t>Dave McMinn</t>
   </si>
   <si>
+    <t>Single Stableford</t>
+  </si>
+  <si>
     <t>Paul Mellor</t>
   </si>
   <si>
@@ -80,6 +83,9 @@
   </si>
   <si>
     <t>Ben Gregory</t>
+  </si>
+  <si>
+    <t>Test Stabelford</t>
   </si>
 </sst>
 </file>
@@ -252,7 +258,7 @@
       <alignment vertical="bottom"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
@@ -292,7 +298,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="8" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
@@ -302,9 +308,6 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1433,11 +1436,13 @@
       <c r="E2" s="8">
         <v>17</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" t="s" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="3" ht="13.55" customHeight="1">
       <c r="A3" t="s" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B3" s="8">
         <v>36</v>
@@ -1449,11 +1454,13 @@
       <c r="E3" s="8">
         <v>16</v>
       </c>
-      <c r="F3" s="4"/>
+      <c r="F3" t="s" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
       <c r="A4" t="s" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B4" s="8">
         <v>35</v>
@@ -1465,11 +1472,13 @@
       <c r="E4" s="8">
         <v>15</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" t="s" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" ht="13.55" customHeight="1">
       <c r="A5" t="s" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B5" s="8">
         <v>35</v>
@@ -1481,11 +1490,13 @@
       <c r="E5" s="8">
         <v>14</v>
       </c>
-      <c r="F5" s="4"/>
+      <c r="F5" t="s" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" ht="13.55" customHeight="1">
       <c r="A6" t="s" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B6" s="8">
         <v>33</v>
@@ -1497,11 +1508,13 @@
       <c r="E6" s="8">
         <v>13</v>
       </c>
-      <c r="F6" s="4"/>
+      <c r="F6" t="s" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" ht="13.55" customHeight="1">
       <c r="A7" t="s" s="10">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B7" s="11">
         <v>32</v>
@@ -1510,14 +1523,16 @@
       <c r="D7" s="11">
         <v>6</v>
       </c>
-      <c r="E7" s="11">
+      <c r="E7" s="13">
         <v>12</v>
       </c>
-      <c r="F7" s="13"/>
+      <c r="F7" t="s" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="8" ht="13.55" customHeight="1">
       <c r="A8" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" s="8">
         <v>30</v>
@@ -1529,11 +1544,13 @@
       <c r="E8" s="8">
         <v>11</v>
       </c>
-      <c r="F8" s="9"/>
+      <c r="F8" t="s" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="9" ht="13.55" customHeight="1">
       <c r="A9" t="s" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B9" s="8">
         <v>30</v>
@@ -1545,11 +1562,13 @@
       <c r="E9" s="8">
         <v>10</v>
       </c>
-      <c r="F9" s="9"/>
+      <c r="F9" t="s" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" ht="13.55" customHeight="1">
       <c r="A10" t="s" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B10" s="8">
         <v>30</v>
@@ -1561,11 +1580,13 @@
       <c r="E10" s="8">
         <v>9</v>
       </c>
-      <c r="F10" s="9"/>
+      <c r="F10" t="s" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="11" ht="13.55" customHeight="1">
       <c r="A11" t="s" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B11" s="8">
         <v>37</v>
@@ -1577,11 +1598,13 @@
       <c r="E11" s="8">
         <v>8</v>
       </c>
-      <c r="F11" s="9"/>
+      <c r="F11" t="s" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="12" ht="13.55" customHeight="1">
       <c r="A12" t="s" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" s="8">
         <v>37</v>
@@ -1593,11 +1616,13 @@
       <c r="E12" s="8">
         <v>7</v>
       </c>
-      <c r="F12" s="9"/>
+      <c r="F12" t="s" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="13" ht="13.55" customHeight="1">
       <c r="A13" t="s" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B13" s="8">
         <v>27</v>
@@ -1609,11 +1634,13 @@
       <c r="E13" s="8">
         <v>6</v>
       </c>
-      <c r="F13" s="9"/>
+      <c r="F13" t="s" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="14" ht="13.55" customHeight="1">
       <c r="A14" t="s" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B14" s="8">
         <v>26</v>
@@ -1625,11 +1652,13 @@
       <c r="E14" s="8">
         <v>5</v>
       </c>
-      <c r="F14" s="9"/>
+      <c r="F14" t="s" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="15" ht="13.55" customHeight="1">
       <c r="A15" t="s" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B15" s="8">
         <v>24</v>
@@ -1641,11 +1670,13 @@
       <c r="E15" s="8">
         <v>4</v>
       </c>
-      <c r="F15" s="9"/>
+      <c r="F15" t="s" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="16" ht="13.55" customHeight="1">
       <c r="A16" t="s" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B16" s="8">
         <v>23</v>
@@ -1657,11 +1688,13 @@
       <c r="E16" s="8">
         <v>3</v>
       </c>
-      <c r="F16" s="9"/>
+      <c r="F16" t="s" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="17" ht="13.55" customHeight="1">
       <c r="A17" t="s" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B17" s="8">
         <v>21</v>
@@ -1673,11 +1706,13 @@
       <c r="E17" s="8">
         <v>2</v>
       </c>
-      <c r="F17" s="9"/>
+      <c r="F17" t="s" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="18" ht="13.55" customHeight="1">
       <c r="A18" t="s" s="14">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B18" s="15">
         <v>10</v>
@@ -1689,7 +1724,9 @@
       <c r="E18" s="8">
         <v>1</v>
       </c>
-      <c r="F18" s="9"/>
+      <c r="F18" t="s" s="4">
+        <v>7</v>
+      </c>
     </row>
     <row r="19" ht="13.55" customHeight="1">
       <c r="A19" t="s" s="5">
@@ -1705,11 +1742,13 @@
       <c r="E19" s="8">
         <v>17</v>
       </c>
-      <c r="F19" s="9"/>
+      <c r="F19" t="s" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="20" ht="13.55" customHeight="1">
       <c r="A20" t="s" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B20" s="8">
         <v>36</v>
@@ -1721,11 +1760,13 @@
       <c r="E20" s="8">
         <v>16</v>
       </c>
-      <c r="F20" s="9"/>
+      <c r="F20" t="s" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="21" ht="13.55" customHeight="1">
       <c r="A21" t="s" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B21" s="8">
         <v>35</v>
@@ -1737,11 +1778,13 @@
       <c r="E21" s="8">
         <v>15</v>
       </c>
-      <c r="F21" s="9"/>
+      <c r="F21" t="s" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="22" ht="13.55" customHeight="1">
       <c r="A22" t="s" s="4">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B22" s="8">
         <v>35</v>
@@ -1753,11 +1796,13 @@
       <c r="E22" s="8">
         <v>14</v>
       </c>
-      <c r="F22" s="9"/>
+      <c r="F22" t="s" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="23" ht="13.55" customHeight="1">
       <c r="A23" t="s" s="4">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B23" s="8">
         <v>33</v>
@@ -1769,11 +1814,13 @@
       <c r="E23" s="8">
         <v>13</v>
       </c>
-      <c r="F23" s="9"/>
+      <c r="F23" t="s" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="24" ht="13.55" customHeight="1">
       <c r="A24" t="s" s="10">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B24" s="11">
         <v>32</v>
@@ -1782,14 +1829,16 @@
       <c r="D24" s="11">
         <v>6</v>
       </c>
-      <c r="E24" s="17">
+      <c r="E24" s="13">
         <v>12</v>
       </c>
-      <c r="F24" s="9"/>
+      <c r="F24" t="s" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="25" ht="13.55" customHeight="1">
       <c r="A25" t="s" s="4">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B25" s="8">
         <v>30</v>
@@ -1801,11 +1850,13 @@
       <c r="E25" s="8">
         <v>11</v>
       </c>
-      <c r="F25" s="9"/>
+      <c r="F25" t="s" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="26" ht="13.55" customHeight="1">
       <c r="A26" t="s" s="4">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B26" s="8">
         <v>30</v>
@@ -1817,11 +1868,13 @@
       <c r="E26" s="8">
         <v>10</v>
       </c>
-      <c r="F26" s="9"/>
+      <c r="F26" t="s" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="27" ht="13.55" customHeight="1">
       <c r="A27" t="s" s="4">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B27" s="8">
         <v>30</v>
@@ -1833,11 +1886,13 @@
       <c r="E27" s="8">
         <v>9</v>
       </c>
-      <c r="F27" s="9"/>
+      <c r="F27" t="s" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="28" ht="13.55" customHeight="1">
       <c r="A28" t="s" s="4">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B28" s="8">
         <v>37</v>
@@ -1849,11 +1904,13 @@
       <c r="E28" s="8">
         <v>8</v>
       </c>
-      <c r="F28" s="9"/>
+      <c r="F28" t="s" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="29" ht="13.55" customHeight="1">
       <c r="A29" t="s" s="4">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B29" s="8">
         <v>37</v>
@@ -1865,11 +1922,13 @@
       <c r="E29" s="8">
         <v>7</v>
       </c>
-      <c r="F29" s="9"/>
+      <c r="F29" t="s" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="30" ht="13.55" customHeight="1">
       <c r="A30" t="s" s="4">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B30" s="8">
         <v>27</v>
@@ -1881,11 +1940,13 @@
       <c r="E30" s="8">
         <v>6</v>
       </c>
-      <c r="F30" s="9"/>
+      <c r="F30" t="s" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="31" ht="13.55" customHeight="1">
       <c r="A31" t="s" s="4">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B31" s="8">
         <v>26</v>
@@ -1897,11 +1958,13 @@
       <c r="E31" s="8">
         <v>5</v>
       </c>
-      <c r="F31" s="9"/>
+      <c r="F31" t="s" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="32" ht="13.55" customHeight="1">
       <c r="A32" t="s" s="4">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B32" s="8">
         <v>24</v>
@@ -1913,11 +1976,13 @@
       <c r="E32" s="8">
         <v>4</v>
       </c>
-      <c r="F32" s="9"/>
+      <c r="F32" t="s" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="33" ht="13.55" customHeight="1">
       <c r="A33" t="s" s="4">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B33" s="8">
         <v>23</v>
@@ -1929,11 +1994,13 @@
       <c r="E33" s="8">
         <v>3</v>
       </c>
-      <c r="F33" s="9"/>
+      <c r="F33" t="s" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="34" ht="13.55" customHeight="1">
       <c r="A34" t="s" s="4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B34" s="8">
         <v>21</v>
@@ -1945,11 +2012,13 @@
       <c r="E34" s="8">
         <v>2</v>
       </c>
-      <c r="F34" s="9"/>
+      <c r="F34" t="s" s="4">
+        <v>24</v>
+      </c>
     </row>
     <row r="35" ht="13.55" customHeight="1">
       <c r="A35" t="s" s="4">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B35" s="8">
         <v>10</v>
@@ -1961,7 +2030,9 @@
       <c r="E35" s="8">
         <v>1</v>
       </c>
-      <c r="F35" s="9"/>
+      <c r="F35" t="s" s="4">
+        <v>24</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Adding 18 or 9 Hole logic and Strokplay / Stableford
</commit_message>
<xml_diff>
--- a/data/leaguedata.xlsx
+++ b/data/leaguedata.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="59">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -51,6 +51,9 @@
     <t xml:space="preserve">Title</t>
   </si>
   <si>
+    <t xml:space="preserve">Type</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dave McMinn</t>
   </si>
   <si>
@@ -63,6 +66,9 @@
     <t xml:space="preserve">Single Stableford</t>
   </si>
   <si>
+    <t xml:space="preserve">18H Stableford</t>
+  </si>
+  <si>
     <t xml:space="preserve">Paul Mellor</t>
   </si>
   <si>
@@ -151,6 +157,9 @@
   </si>
   <si>
     <t xml:space="preserve">1st Monthly Medal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">18H Strokeplay</t>
   </si>
   <si>
     <t xml:space="preserve">Dan Edmiston</t>
@@ -291,7 +300,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -310,6 +319,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -529,10 +542,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:K39"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2:B18"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J39" activeCellId="0" sqref="J39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -545,7 +558,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="7.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="31.85"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="10" style="1" width="8.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="23.41"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="11" style="1" width="8.85"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -576,10 +590,13 @@
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>62</v>
@@ -594,24 +611,27 @@
         <v>17</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="4" t="n">
         <v>24.48</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="4" t="n">
         <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>64</v>
@@ -626,24 +646,27 @@
         <v>16</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="G3" s="4" t="n">
         <v>16.32</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J3" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" s="4" t="n">
         <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B4" s="4" t="n">
         <v>66</v>
@@ -658,22 +681,25 @@
         <v>15</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G4" s="4"/>
       <c r="H4" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J4" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K4" s="4" t="n">
         <v>66</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>66</v>
@@ -688,22 +714,25 @@
         <v>14</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="G5" s="4"/>
       <c r="H5" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J5" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K5" s="4" t="n">
         <v>66</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>67</v>
@@ -718,22 +747,25 @@
         <v>13</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="G6" s="4"/>
       <c r="H6" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K6" s="4" t="n">
         <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>68</v>
@@ -748,22 +780,25 @@
         <v>12</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="G7" s="4"/>
       <c r="H7" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J7" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K7" s="4" t="n">
         <v>68</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B8" s="4" t="n">
         <v>71</v>
@@ -778,22 +813,25 @@
         <v>11</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G8" s="4"/>
       <c r="H8" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J8" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K8" s="4" t="n">
         <v>71</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B9" s="4" t="n">
         <v>71</v>
@@ -808,22 +846,25 @@
         <v>10</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G9" s="4"/>
       <c r="H9" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J9" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K9" s="4" t="n">
         <v>71</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B10" s="4" t="n">
         <v>72</v>
@@ -838,22 +879,25 @@
         <v>9</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J10" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K10" s="4" t="n">
         <v>72</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B11" s="4" t="n">
         <v>73</v>
@@ -868,22 +912,25 @@
         <v>8</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G11" s="4"/>
       <c r="H11" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J11" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K11" s="4" t="n">
         <v>73</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B12" s="4" t="n">
         <v>73</v>
@@ -898,22 +945,25 @@
         <v>7</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G12" s="4"/>
       <c r="H12" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J12" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K12" s="4" t="n">
         <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B13" s="4" t="n">
         <v>73</v>
@@ -928,22 +978,25 @@
         <v>6</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="G13" s="4"/>
       <c r="H13" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J13" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K13" s="4" t="n">
         <v>73</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B14" s="4" t="n">
         <v>74</v>
@@ -958,22 +1011,25 @@
         <v>5</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="G14" s="4"/>
       <c r="H14" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I14" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J14" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K14" s="4" t="n">
         <v>74</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B15" s="4" t="n">
         <v>76</v>
@@ -988,22 +1044,25 @@
         <v>4</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J15" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="4" t="n">
         <v>76</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B16" s="4" t="n">
         <v>77</v>
@@ -1018,22 +1077,25 @@
         <v>3</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="G16" s="4"/>
       <c r="H16" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J16" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K16" s="4" t="n">
         <v>77</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B17" s="4" t="n">
         <v>80</v>
@@ -1048,22 +1110,25 @@
         <v>2</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="G17" s="4"/>
       <c r="H17" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J17" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K17" s="4" t="n">
         <v>80</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B18" s="4" t="n">
         <v>91</v>
@@ -1078,22 +1143,25 @@
         <v>1</v>
       </c>
       <c r="F18" s="3" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J18" s="4" t="n">
+        <v>13</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="K18" s="4" t="n">
         <v>91</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="3" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B19" s="4" t="n">
         <v>59</v>
@@ -1106,21 +1174,24 @@
         <v>21</v>
       </c>
       <c r="F19" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G19" s="4" t="n">
         <v>30.24</v>
       </c>
       <c r="H19" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B20" s="4" t="n">
         <v>61</v>
@@ -1133,21 +1204,24 @@
         <v>20</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G20" s="4" t="n">
         <v>20.16</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I20" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="3" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B21" s="4" t="n">
         <v>63</v>
@@ -1160,19 +1234,22 @@
         <v>19</v>
       </c>
       <c r="F21" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G21" s="4"/>
       <c r="H21" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="3" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B22" s="4" t="n">
         <v>63</v>
@@ -1185,19 +1262,22 @@
         <v>18</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G22" s="4"/>
       <c r="H22" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I22" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B23" s="4" t="n">
         <v>64</v>
@@ -1210,19 +1290,22 @@
         <v>17</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G23" s="4"/>
       <c r="H23" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I23" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="3" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B24" s="4" t="n">
         <v>64</v>
@@ -1235,19 +1318,22 @@
         <v>16</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G24" s="4"/>
       <c r="H24" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B25" s="4" t="n">
         <v>65</v>
@@ -1260,19 +1346,22 @@
         <v>15</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G25" s="4"/>
       <c r="H25" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J25" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B26" s="4" t="n">
         <v>65</v>
@@ -1285,19 +1374,22 @@
         <v>14</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G26" s="4"/>
       <c r="H26" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B27" s="4" t="n">
         <v>66</v>
@@ -1310,19 +1402,22 @@
         <v>13</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G27" s="4"/>
       <c r="H27" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B28" s="4" t="n">
         <v>68</v>
@@ -1335,19 +1430,22 @@
         <v>12</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G28" s="4"/>
       <c r="H28" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J28" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="3" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B29" s="4" t="n">
         <v>69</v>
@@ -1360,19 +1458,22 @@
         <v>11</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G29" s="4"/>
       <c r="H29" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I29" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="3" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B30" s="4" t="n">
         <v>70</v>
@@ -1385,19 +1486,22 @@
         <v>10</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G30" s="4"/>
       <c r="H30" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J30" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B31" s="4" t="n">
         <v>70</v>
@@ -1410,19 +1514,22 @@
         <v>9</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G31" s="4"/>
       <c r="H31" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="3" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B32" s="4" t="n">
         <v>71</v>
@@ -1435,19 +1542,22 @@
         <v>8</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G32" s="4"/>
       <c r="H32" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B33" s="4" t="n">
         <v>72</v>
@@ -1460,19 +1570,22 @@
         <v>7</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G33" s="4"/>
       <c r="H33" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B34" s="4" t="n">
         <v>72</v>
@@ -1485,19 +1598,22 @@
         <v>6</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G34" s="4"/>
       <c r="H34" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B35" s="4" t="n">
         <v>73</v>
@@ -1510,19 +1626,22 @@
         <v>5</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G35" s="4"/>
       <c r="H35" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="3" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B36" s="4" t="n">
         <v>76</v>
@@ -1535,19 +1654,22 @@
         <v>4</v>
       </c>
       <c r="F36" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G36" s="4"/>
       <c r="H36" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="3" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B37" s="4" t="n">
         <v>77</v>
@@ -1560,19 +1682,22 @@
         <v>3</v>
       </c>
       <c r="F37" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G37" s="4"/>
       <c r="H37" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="3" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B38" s="4" t="n">
         <v>77</v>
@@ -1585,19 +1710,22 @@
         <v>2</v>
       </c>
       <c r="F38" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G38" s="4"/>
       <c r="H38" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="3" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B39" s="4" t="n">
         <v>80</v>
@@ -1610,14 +1738,17 @@
         <v>1</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="G39" s="4"/>
       <c r="H39" s="3" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -1643,102 +1774,102 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="B2:B18 A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="J39 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3515625" defaultRowHeight="17.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="5" width="16.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="6" width="16.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="A1" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" customFormat="false" ht="15.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="B2" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
     </row>
     <row r="3" customFormat="false" ht="15.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="9" t="s">
-        <v>32</v>
-      </c>
-      <c r="B3" s="10" t="n">
+      <c r="A3" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="B3" s="11" t="n">
         <v>12.7</v>
       </c>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
+      <c r="C3" s="11"/>
+      <c r="D3" s="11"/>
+      <c r="E3" s="11"/>
     </row>
     <row r="4" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11"/>
-      <c r="C4" s="11"/>
-      <c r="D4" s="11"/>
-      <c r="E4" s="11"/>
+      <c r="A4" s="11"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
     </row>
     <row r="5" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="10"/>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
     </row>
     <row r="6" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11"/>
-      <c r="C6" s="11"/>
-      <c r="D6" s="11"/>
-      <c r="E6" s="11"/>
+      <c r="A6" s="11"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
     </row>
     <row r="7" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="10"/>
-      <c r="B7" s="10"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
+      <c r="A7" s="11"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
+      <c r="A8" s="11"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
     </row>
     <row r="9" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="10"/>
-      <c r="B9" s="10"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="10"/>
-      <c r="E9" s="10"/>
+      <c r="A9" s="11"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="10"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
+      <c r="A10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
     </row>
     <row r="11" customFormat="false" ht="15.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
+      <c r="A11" s="11"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1762,7 +1893,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="B2:B18 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="J39 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1774,10 +1905,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -1785,10 +1916,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1796,10 +1927,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>

</xml_diff>

<commit_message>
Pro's Roll up test data
</commit_message>
<xml_diff>
--- a/data/leaguedata.xlsx
+++ b/data/leaguedata.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="63">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -172,6 +172,45 @@
   </si>
   <si>
     <t xml:space="preserve">Matt Withers</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Pro’s Roll Up – Week 1 -  17</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">th</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> April</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">17/04/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pro’s Roll Up – Week 1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9H Stableford</t>
   </si>
   <si>
     <t xml:space="preserve">Table 1</t>
@@ -209,7 +248,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -239,13 +278,20 @@
       <charset val="1"/>
     </font>
     <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
       <sz val="12"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +302,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFB2B2B2"/>
+        <bgColor rgb="FF969696"/>
       </patternFill>
     </fill>
   </fills>
@@ -300,7 +352,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -321,15 +373,39 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -362,6 +438,66 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008000"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FF808000"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FFB2B2B2"/>
+      <rgbColor rgb="FF808080"/>
+      <rgbColor rgb="FF9999FF"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FFFFFFCC"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FF660066"/>
+      <rgbColor rgb="FFFF8080"/>
+      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FFCCCCFF"/>
+      <rgbColor rgb="FF000080"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF800080"/>
+      <rgbColor rgb="FF800000"/>
+      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FF00CCFF"/>
+      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFCCFFCC"/>
+      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FF99CCFF"/>
+      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFCC99FF"/>
+      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FF3366FF"/>
+      <rgbColor rgb="FF33CCCC"/>
+      <rgbColor rgb="FF99CC00"/>
+      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFF9900"/>
+      <rgbColor rgb="FFFF6600"/>
+      <rgbColor rgb="FF666699"/>
+      <rgbColor rgb="FF969696"/>
+      <rgbColor rgb="FF003366"/>
+      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF003300"/>
+      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FF993366"/>
+      <rgbColor rgb="FF333399"/>
+      <rgbColor rgb="FF333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -542,10 +678,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K39"/>
+  <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J39" activeCellId="0" sqref="J39"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H41" activeCellId="0" sqref="H41:H47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1159,597 +1295,853 @@
         <v>91</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
+    <row r="19" s="9" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B19" s="4" t="n">
+      <c r="B19" s="7" t="n">
         <v>59</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4" t="n">
+      <c r="C19" s="7"/>
+      <c r="D19" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="E19" s="4" t="n">
+      <c r="E19" s="7" t="n">
         <v>21</v>
       </c>
-      <c r="F19" s="3" t="s">
+      <c r="F19" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G19" s="4" t="n">
+      <c r="G19" s="7" t="n">
         <v>30.24</v>
       </c>
-      <c r="H19" s="3" t="s">
+      <c r="H19" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I19" s="3" t="s">
+      <c r="I19" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J19" s="5" t="s">
+      <c r="J19" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3" t="s">
+    <row r="20" s="9" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B20" s="4" t="n">
+      <c r="B20" s="7" t="n">
         <v>61</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4" t="n">
+      <c r="C20" s="7"/>
+      <c r="D20" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="E20" s="4" t="n">
+      <c r="E20" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="F20" s="3" t="s">
+      <c r="F20" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G20" s="4" t="n">
+      <c r="G20" s="7" t="n">
         <v>20.16</v>
       </c>
-      <c r="H20" s="3" t="s">
+      <c r="H20" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I20" s="3" t="s">
+      <c r="I20" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="5" t="s">
+      <c r="J20" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
+    <row r="21" s="9" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="B21" s="4" t="n">
+      <c r="B21" s="7" t="n">
         <v>63</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4" t="n">
+      <c r="C21" s="7"/>
+      <c r="D21" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="E21" s="4" t="n">
+      <c r="E21" s="7" t="n">
         <v>19</v>
       </c>
-      <c r="F21" s="3" t="s">
+      <c r="F21" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G21" s="4"/>
-      <c r="H21" s="3" t="s">
+      <c r="G21" s="7"/>
+      <c r="H21" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I21" s="3" t="s">
+      <c r="I21" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="5" t="s">
+      <c r="J21" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3" t="s">
+    <row r="22" s="9" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="4" t="n">
+      <c r="B22" s="7" t="n">
         <v>63</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4" t="n">
+      <c r="C22" s="7"/>
+      <c r="D22" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="E22" s="4" t="n">
+      <c r="E22" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="F22" s="3" t="s">
+      <c r="F22" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G22" s="4"/>
-      <c r="H22" s="3" t="s">
+      <c r="G22" s="7"/>
+      <c r="H22" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I22" s="3" t="s">
+      <c r="I22" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J22" s="5" t="s">
+      <c r="J22" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="3" t="s">
+    <row r="23" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="4" t="n">
+      <c r="B23" s="7" t="n">
         <v>64</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4" t="n">
+      <c r="C23" s="7"/>
+      <c r="D23" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="E23" s="4" t="n">
+      <c r="E23" s="7" t="n">
         <v>17</v>
       </c>
-      <c r="F23" s="3" t="s">
+      <c r="F23" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G23" s="4"/>
-      <c r="H23" s="3" t="s">
+      <c r="G23" s="7"/>
+      <c r="H23" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I23" s="3" t="s">
+      <c r="I23" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J23" s="5" t="s">
+      <c r="J23" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="3" t="s">
+    <row r="24" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B24" s="4" t="n">
+      <c r="B24" s="7" t="n">
         <v>64</v>
       </c>
-      <c r="C24" s="4"/>
-      <c r="D24" s="4" t="n">
+      <c r="C24" s="7"/>
+      <c r="D24" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="E24" s="4" t="n">
+      <c r="E24" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="F24" s="3" t="s">
+      <c r="F24" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G24" s="4"/>
-      <c r="H24" s="3" t="s">
+      <c r="G24" s="7"/>
+      <c r="H24" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I24" s="3" t="s">
+      <c r="I24" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J24" s="5" t="s">
+      <c r="J24" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="3" t="s">
+    <row r="25" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="4" t="n">
+      <c r="B25" s="7" t="n">
         <v>65</v>
       </c>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4" t="n">
+      <c r="C25" s="7"/>
+      <c r="D25" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="E25" s="4" t="n">
+      <c r="E25" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="F25" s="3" t="s">
+      <c r="F25" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G25" s="4"/>
-      <c r="H25" s="3" t="s">
+      <c r="G25" s="7"/>
+      <c r="H25" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I25" s="3" t="s">
+      <c r="I25" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J25" s="5" t="s">
+      <c r="J25" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="3" t="s">
+    <row r="26" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="4" t="n">
+      <c r="B26" s="7" t="n">
         <v>65</v>
       </c>
-      <c r="C26" s="4"/>
-      <c r="D26" s="4" t="n">
+      <c r="C26" s="7"/>
+      <c r="D26" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="E26" s="4" t="n">
+      <c r="E26" s="7" t="n">
         <v>14</v>
       </c>
-      <c r="F26" s="3" t="s">
+      <c r="F26" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G26" s="4"/>
-      <c r="H26" s="3" t="s">
+      <c r="G26" s="7"/>
+      <c r="H26" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I26" s="3" t="s">
+      <c r="I26" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J26" s="5" t="s">
+      <c r="J26" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="3" t="s">
+    <row r="27" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="4" t="n">
+      <c r="B27" s="7" t="n">
         <v>66</v>
       </c>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4" t="n">
+      <c r="C27" s="7"/>
+      <c r="D27" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="E27" s="4" t="n">
+      <c r="E27" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="F27" s="3" t="s">
+      <c r="F27" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G27" s="4"/>
-      <c r="H27" s="3" t="s">
+      <c r="G27" s="7"/>
+      <c r="H27" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="I27" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J27" s="5" t="s">
+      <c r="J27" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="3" t="s">
+    <row r="28" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="4" t="n">
+      <c r="B28" s="7" t="n">
         <v>68</v>
       </c>
-      <c r="C28" s="4"/>
-      <c r="D28" s="4" t="n">
+      <c r="C28" s="7"/>
+      <c r="D28" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="E28" s="4" t="n">
+      <c r="E28" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="F28" s="3" t="s">
+      <c r="F28" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G28" s="4"/>
-      <c r="H28" s="3" t="s">
+      <c r="G28" s="7"/>
+      <c r="H28" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I28" s="3" t="s">
+      <c r="I28" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J28" s="5" t="s">
+      <c r="J28" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="3" t="s">
+    <row r="29" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B29" s="4" t="n">
+      <c r="B29" s="7" t="n">
         <v>69</v>
       </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4" t="n">
+      <c r="C29" s="7"/>
+      <c r="D29" s="7" t="n">
         <v>11</v>
       </c>
-      <c r="E29" s="4" t="n">
+      <c r="E29" s="7" t="n">
         <v>11</v>
       </c>
-      <c r="F29" s="3" t="s">
+      <c r="F29" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G29" s="4"/>
-      <c r="H29" s="3" t="s">
+      <c r="G29" s="7"/>
+      <c r="H29" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I29" s="3" t="s">
+      <c r="I29" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J29" s="5" t="s">
+      <c r="J29" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="3" t="s">
+    <row r="30" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="4" t="n">
+      <c r="B30" s="7" t="n">
         <v>70</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="4" t="n">
+      <c r="C30" s="7"/>
+      <c r="D30" s="7" t="n">
         <v>12</v>
       </c>
-      <c r="E30" s="4" t="n">
+      <c r="E30" s="7" t="n">
         <v>10</v>
       </c>
-      <c r="F30" s="3" t="s">
+      <c r="F30" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G30" s="4"/>
-      <c r="H30" s="3" t="s">
+      <c r="G30" s="7"/>
+      <c r="H30" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I30" s="3" t="s">
+      <c r="I30" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J30" s="5" t="s">
+      <c r="J30" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="3" t="s">
+    <row r="31" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="4" t="n">
+      <c r="B31" s="7" t="n">
         <v>70</v>
       </c>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4" t="n">
+      <c r="C31" s="7"/>
+      <c r="D31" s="7" t="n">
         <v>13</v>
       </c>
-      <c r="E31" s="4" t="n">
+      <c r="E31" s="7" t="n">
         <v>9</v>
       </c>
-      <c r="F31" s="3" t="s">
+      <c r="F31" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G31" s="4"/>
-      <c r="H31" s="3" t="s">
+      <c r="G31" s="7"/>
+      <c r="H31" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I31" s="3" t="s">
+      <c r="I31" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J31" s="5" t="s">
+      <c r="J31" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="3" t="s">
+    <row r="32" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="4" t="n">
+      <c r="B32" s="7" t="n">
         <v>71</v>
       </c>
-      <c r="C32" s="4"/>
-      <c r="D32" s="4" t="n">
+      <c r="C32" s="7"/>
+      <c r="D32" s="7" t="n">
         <v>14</v>
       </c>
-      <c r="E32" s="4" t="n">
+      <c r="E32" s="7" t="n">
         <v>8</v>
       </c>
-      <c r="F32" s="3" t="s">
+      <c r="F32" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G32" s="4"/>
-      <c r="H32" s="3" t="s">
+      <c r="G32" s="7"/>
+      <c r="H32" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I32" s="3" t="s">
+      <c r="I32" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J32" s="5" t="s">
+      <c r="J32" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="3" t="s">
+    <row r="33" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="4" t="n">
+      <c r="B33" s="7" t="n">
         <v>72</v>
       </c>
-      <c r="C33" s="4"/>
-      <c r="D33" s="4" t="n">
+      <c r="C33" s="7"/>
+      <c r="D33" s="7" t="n">
         <v>15</v>
       </c>
-      <c r="E33" s="4" t="n">
+      <c r="E33" s="7" t="n">
         <v>7</v>
       </c>
-      <c r="F33" s="3" t="s">
+      <c r="F33" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G33" s="4"/>
-      <c r="H33" s="3" t="s">
+      <c r="G33" s="7"/>
+      <c r="H33" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I33" s="3" t="s">
+      <c r="I33" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J33" s="5" t="s">
+      <c r="J33" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="3" t="s">
+    <row r="34" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B34" s="4" t="n">
+      <c r="B34" s="7" t="n">
         <v>72</v>
       </c>
-      <c r="C34" s="4"/>
-      <c r="D34" s="4" t="n">
+      <c r="C34" s="7"/>
+      <c r="D34" s="7" t="n">
         <v>16</v>
       </c>
-      <c r="E34" s="4" t="n">
+      <c r="E34" s="7" t="n">
         <v>6</v>
       </c>
-      <c r="F34" s="3" t="s">
+      <c r="F34" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G34" s="4"/>
-      <c r="H34" s="3" t="s">
+      <c r="G34" s="7"/>
+      <c r="H34" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I34" s="3" t="s">
+      <c r="I34" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J34" s="5" t="s">
+      <c r="J34" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="3" t="s">
+    <row r="35" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="B35" s="4" t="n">
+      <c r="B35" s="7" t="n">
         <v>73</v>
       </c>
-      <c r="C35" s="4"/>
-      <c r="D35" s="4" t="n">
+      <c r="C35" s="7"/>
+      <c r="D35" s="7" t="n">
         <v>17</v>
       </c>
-      <c r="E35" s="4" t="n">
+      <c r="E35" s="7" t="n">
         <v>5</v>
       </c>
-      <c r="F35" s="3" t="s">
+      <c r="F35" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G35" s="4"/>
-      <c r="H35" s="3" t="s">
+      <c r="G35" s="7"/>
+      <c r="H35" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I35" s="3" t="s">
+      <c r="I35" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J35" s="5" t="s">
+      <c r="J35" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="3" t="s">
+    <row r="36" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B36" s="4" t="n">
+      <c r="B36" s="7" t="n">
         <v>76</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4" t="n">
+      <c r="C36" s="7"/>
+      <c r="D36" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="E36" s="4" t="n">
+      <c r="E36" s="7" t="n">
         <v>4</v>
       </c>
-      <c r="F36" s="3" t="s">
+      <c r="F36" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G36" s="4"/>
-      <c r="H36" s="3" t="s">
+      <c r="G36" s="7"/>
+      <c r="H36" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I36" s="3" t="s">
+      <c r="I36" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J36" s="5" t="s">
+      <c r="J36" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="3" t="s">
+    <row r="37" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B37" s="4" t="n">
+      <c r="B37" s="7" t="n">
         <v>77</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="4" t="n">
+      <c r="C37" s="7"/>
+      <c r="D37" s="7" t="n">
         <v>19</v>
       </c>
-      <c r="E37" s="4" t="n">
+      <c r="E37" s="7" t="n">
         <v>3</v>
       </c>
-      <c r="F37" s="3" t="s">
+      <c r="F37" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G37" s="4"/>
-      <c r="H37" s="3" t="s">
+      <c r="G37" s="7"/>
+      <c r="H37" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I37" s="3" t="s">
+      <c r="I37" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J37" s="5" t="s">
+      <c r="J37" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="3" t="s">
+    <row r="38" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="4" t="n">
+      <c r="B38" s="7" t="n">
         <v>77</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="4" t="n">
+      <c r="C38" s="7"/>
+      <c r="D38" s="7" t="n">
         <v>20</v>
       </c>
-      <c r="E38" s="4" t="n">
+      <c r="E38" s="7" t="n">
         <v>2</v>
       </c>
-      <c r="F38" s="3" t="s">
+      <c r="F38" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G38" s="4"/>
-      <c r="H38" s="3" t="s">
+      <c r="G38" s="7"/>
+      <c r="H38" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I38" s="3" t="s">
+      <c r="I38" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J38" s="5" t="s">
+      <c r="J38" s="8" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="3" t="s">
+    <row r="39" s="9" customFormat="true" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B39" s="4" t="n">
+      <c r="B39" s="7" t="n">
         <v>80</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4" t="n">
+      <c r="C39" s="7"/>
+      <c r="D39" s="7" t="n">
         <v>21</v>
       </c>
-      <c r="E39" s="4" t="n">
+      <c r="E39" s="7" t="n">
         <v>1</v>
       </c>
-      <c r="F39" s="3" t="s">
+      <c r="F39" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="G39" s="4"/>
-      <c r="H39" s="3" t="s">
+      <c r="G39" s="7"/>
+      <c r="H39" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="I39" s="3" t="s">
+      <c r="I39" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="J39" s="5" t="s">
+      <c r="J39" s="8" t="s">
         <v>45</v>
       </c>
+    </row>
+    <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B40" s="10"/>
+      <c r="C40" s="10" t="n">
+        <v>22</v>
+      </c>
+      <c r="D40" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G40" s="10" t="n">
+        <v>100</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I40" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J40" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="10"/>
+      <c r="C41" s="10" t="n">
+        <v>22</v>
+      </c>
+      <c r="D41" s="11" t="n">
+        <v>2</v>
+      </c>
+      <c r="E41" s="10" t="n">
+        <v>7</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G41" s="10" t="n">
+        <v>50</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I41" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J41" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" s="10"/>
+      <c r="C42" s="10" t="n">
+        <v>18</v>
+      </c>
+      <c r="D42" s="11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E42" s="10" t="n">
+        <v>6</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G42" s="10"/>
+      <c r="H42" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I42" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B43" s="10"/>
+      <c r="C43" s="10" t="n">
+        <v>18</v>
+      </c>
+      <c r="D43" s="11" t="n">
+        <v>4</v>
+      </c>
+      <c r="E43" s="10" t="n">
+        <v>5</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G43" s="10"/>
+      <c r="H43" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I43" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J43" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B44" s="10"/>
+      <c r="C44" s="10" t="n">
+        <v>17</v>
+      </c>
+      <c r="D44" s="11" t="n">
+        <v>5</v>
+      </c>
+      <c r="E44" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G44" s="10"/>
+      <c r="H44" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I44" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B45" s="10"/>
+      <c r="C45" s="10" t="n">
+        <v>16</v>
+      </c>
+      <c r="D45" s="11" t="n">
+        <v>6</v>
+      </c>
+      <c r="E45" s="10" t="n">
+        <v>3</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G45" s="10"/>
+      <c r="H45" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J45" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10" t="n">
+        <v>15</v>
+      </c>
+      <c r="D46" s="11" t="n">
+        <v>7</v>
+      </c>
+      <c r="E46" s="10" t="n">
+        <v>2</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J46" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B47" s="10"/>
+      <c r="C47" s="10" t="n">
+        <v>13</v>
+      </c>
+      <c r="D47" s="11" t="n">
+        <v>8</v>
+      </c>
+      <c r="E47" s="10" t="n">
+        <v>1</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="G47" s="10"/>
+      <c r="H47" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="J47" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="3"/>
+      <c r="J48" s="10"/>
+    </row>
+    <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="3"/>
+    </row>
+    <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="3"/>
+    </row>
+    <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="3"/>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="3"/>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="3"/>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="3"/>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="3"/>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="3"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1774,102 +2166,102 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="J39 A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="H41:H47 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3515625" defaultRowHeight="17.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="6" width="16.35"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="1" style="12" width="16.35"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="26.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="A1" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
     </row>
     <row r="2" customFormat="false" ht="15.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="B2" s="14" t="s">
+        <v>55</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
     </row>
     <row r="3" customFormat="false" ht="15.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="B3" s="11" t="n">
+      <c r="B3" s="17" t="n">
         <v>12.7</v>
       </c>
-      <c r="C3" s="11"/>
-      <c r="D3" s="11"/>
-      <c r="E3" s="11"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
     </row>
     <row r="4" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="11"/>
-      <c r="B4" s="12"/>
-      <c r="C4" s="12"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="12"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="18"/>
+      <c r="C4" s="18"/>
+      <c r="D4" s="18"/>
+      <c r="E4" s="18"/>
     </row>
     <row r="5" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="11"/>
-      <c r="B5" s="11"/>
-      <c r="C5" s="11"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
     </row>
     <row r="6" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="11"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
+      <c r="A6" s="17"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
     </row>
     <row r="7" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="11"/>
-      <c r="B7" s="11"/>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
+      <c r="A7" s="17"/>
+      <c r="B7" s="17"/>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
     </row>
     <row r="8" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="11"/>
-      <c r="B8" s="12"/>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
-      <c r="E8" s="12"/>
+      <c r="A8" s="17"/>
+      <c r="B8" s="18"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
     </row>
     <row r="9" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
     </row>
     <row r="10" customFormat="false" ht="14.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="11"/>
-      <c r="B10" s="12"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
     </row>
     <row r="11" customFormat="false" ht="15.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="11"/>
-      <c r="B11" s="11"/>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
+      <c r="A11" s="17"/>
+      <c r="B11" s="17"/>
+      <c r="C11" s="17"/>
+      <c r="D11" s="17"/>
+      <c r="E11" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1893,7 +2285,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="J39 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H41:H47 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1905,10 +2297,10 @@
   <sheetData>
     <row r="1" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4"/>
@@ -1916,10 +2308,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
@@ -1927,10 +2319,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>

</xml_diff>

<commit_message>
Total Winnings fix for 9h stableford comps
</commit_message>
<xml_diff>
--- a/data/leaguedata.xlsx
+++ b/data/leaguedata.xlsx
@@ -207,7 +207,7 @@
     <t xml:space="preserve">17/04/2025</t>
   </si>
   <si>
-    <t xml:space="preserve">Pro’s Roll Up – Week 1</t>
+    <t xml:space="preserve">Pro’s Roll Up – Stableford - **TEST DATA**</t>
   </si>
   <si>
     <t xml:space="preserve">9H Stableford</t>
@@ -397,7 +397,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -680,8 +680,8 @@
   </sheetPr>
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A26" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H41" activeCellId="0" sqref="H41:H47"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I48" activeCellId="0" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1891,7 +1891,9 @@
       <c r="A40" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B40" s="10"/>
+      <c r="B40" s="10" t="n">
+        <v>34</v>
+      </c>
       <c r="C40" s="10" t="n">
         <v>22</v>
       </c>
@@ -1921,7 +1923,9 @@
       <c r="A41" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B41" s="10"/>
+      <c r="B41" s="11" t="n">
+        <v>38</v>
+      </c>
       <c r="C41" s="10" t="n">
         <v>22</v>
       </c>
@@ -1951,7 +1955,9 @@
       <c r="A42" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B42" s="10"/>
+      <c r="B42" s="11" t="n">
+        <v>41</v>
+      </c>
       <c r="C42" s="10" t="n">
         <v>18</v>
       </c>
@@ -1979,7 +1985,9 @@
       <c r="A43" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="10"/>
+      <c r="B43" s="11" t="n">
+        <v>39</v>
+      </c>
       <c r="C43" s="10" t="n">
         <v>18</v>
       </c>
@@ -2007,7 +2015,9 @@
       <c r="A44" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B44" s="10"/>
+      <c r="B44" s="11" t="n">
+        <v>34</v>
+      </c>
       <c r="C44" s="10" t="n">
         <v>17</v>
       </c>
@@ -2035,7 +2045,9 @@
       <c r="A45" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B45" s="10"/>
+      <c r="B45" s="11" t="n">
+        <v>34</v>
+      </c>
       <c r="C45" s="10" t="n">
         <v>16</v>
       </c>
@@ -2063,7 +2075,9 @@
       <c r="A46" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B46" s="10"/>
+      <c r="B46" s="11" t="n">
+        <v>40</v>
+      </c>
       <c r="C46" s="10" t="n">
         <v>15</v>
       </c>
@@ -2091,7 +2105,9 @@
       <c r="A47" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B47" s="10"/>
+      <c r="B47" s="11" t="n">
+        <v>24</v>
+      </c>
       <c r="C47" s="10" t="n">
         <v>13</v>
       </c>
@@ -2166,7 +2182,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A1" activeCellId="1" sqref="H41:H47 A1"/>
+      <selection pane="bottomRight" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3515625" defaultRowHeight="17.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2285,7 +2301,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H41:H47 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Pros Roll Up Week1
Data Uploaded
</commit_message>
<xml_diff>
--- a/data/leaguedata.xlsx
+++ b/data/leaguedata.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="69">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -191,12 +191,27 @@
     <t xml:space="preserve">19.20</t>
   </si>
   <si>
-    <t xml:space="preserve">N/R</t>
-  </si>
-  <si>
     <t xml:space="preserve">Centenary Trophy – N/R</t>
   </si>
   <si>
+    <t xml:space="preserve">Pros Roll Up Week 2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24/04/2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pros Roll Up Week 2 – Stableford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9H Stableford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7.68</t>
+  </si>
+  <si>
     <t xml:space="preserve">Key</t>
   </si>
   <si>
@@ -206,13 +221,13 @@
     <t xml:space="preserve">League Champions Pot</t>
   </si>
   <si>
-    <t xml:space="preserve">34.80</t>
+    <t xml:space="preserve">44.60</t>
   </si>
   <si>
     <t xml:space="preserve">Next Competition</t>
   </si>
   <si>
-    <t xml:space="preserve">Pros Roll Up Week 2 24/04/2025</t>
+    <t xml:space="preserve">Jubilee Bowl Stableford | 26/04/2025</t>
   </si>
 </sst>
 </file>
@@ -223,7 +238,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -252,8 +267,15 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -276,6 +298,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB3CAC7"/>
         <bgColor rgb="FFB2B2B2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF395511"/>
+        <bgColor rgb="FF333333"/>
       </patternFill>
     </fill>
   </fills>
@@ -320,7 +348,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="24">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -389,6 +417,34 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -451,7 +507,7 @@
       <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
-      <rgbColor rgb="FF333300"/>
+      <rgbColor rgb="FF395511"/>
       <rgbColor rgb="FF993300"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
@@ -638,10 +694,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K59"/>
+  <dimension ref="A1:K67"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A65" activeCellId="0" sqref="A65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2387,8 +2443,8 @@
       <c r="A59" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="B59" s="14" t="s">
-        <v>56</v>
+      <c r="B59" s="14" t="n">
+        <v>0</v>
       </c>
       <c r="C59" s="14"/>
       <c r="D59" s="14" t="n">
@@ -2398,7 +2454,7 @@
         <v>1</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G59" s="16"/>
       <c r="H59" s="14" t="s">
@@ -2409,6 +2465,250 @@
       </c>
       <c r="J59" s="15" t="s">
         <v>46</v>
+      </c>
+    </row>
+    <row r="60" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="B60" s="17" t="n">
+        <v>38</v>
+      </c>
+      <c r="C60" s="17" t="n">
+        <v>19</v>
+      </c>
+      <c r="D60" s="17" t="n">
+        <v>1</v>
+      </c>
+      <c r="E60" s="17" t="n">
+        <v>8</v>
+      </c>
+      <c r="F60" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G60" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="H60" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I60" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J60" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="61" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="B61" s="17" t="n">
+        <v>39</v>
+      </c>
+      <c r="C61" s="17" t="n">
+        <v>18</v>
+      </c>
+      <c r="D61" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="E61" s="17" t="n">
+        <v>7</v>
+      </c>
+      <c r="F61" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G61" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="H61" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I61" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J61" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="62" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="B62" s="17" t="n">
+        <v>39</v>
+      </c>
+      <c r="C62" s="17" t="n">
+        <v>18</v>
+      </c>
+      <c r="D62" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="E62" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="F62" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G62" s="18"/>
+      <c r="H62" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I62" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J62" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="B63" s="17" t="n">
+        <v>42</v>
+      </c>
+      <c r="C63" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="D63" s="17" t="n">
+        <v>4</v>
+      </c>
+      <c r="E63" s="17" t="n">
+        <v>5</v>
+      </c>
+      <c r="F63" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G63" s="18"/>
+      <c r="H63" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I63" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J63" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="64" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="B64" s="20" t="n">
+        <v>40</v>
+      </c>
+      <c r="C64" s="20" t="n">
+        <v>17</v>
+      </c>
+      <c r="D64" s="20" t="n">
+        <v>5</v>
+      </c>
+      <c r="E64" s="20" t="n">
+        <v>4</v>
+      </c>
+      <c r="F64" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G64" s="21"/>
+      <c r="H64" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="I64" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="J64" s="20" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="65" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="B65" s="17" t="n">
+        <v>38</v>
+      </c>
+      <c r="C65" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="D65" s="17" t="n">
+        <v>6</v>
+      </c>
+      <c r="E65" s="17" t="n">
+        <v>3</v>
+      </c>
+      <c r="F65" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G65" s="18"/>
+      <c r="H65" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I65" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J65" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" s="19" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="B66" s="17" t="n">
+        <v>42</v>
+      </c>
+      <c r="C66" s="17" t="n">
+        <v>17</v>
+      </c>
+      <c r="D66" s="17" t="n">
+        <v>7</v>
+      </c>
+      <c r="E66" s="17" t="n">
+        <v>2</v>
+      </c>
+      <c r="F66" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="G66" s="18"/>
+      <c r="H66" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="I66" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="J66" s="17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="67" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B67" s="20" t="n">
+        <v>40</v>
+      </c>
+      <c r="C67" s="20" t="n">
+        <v>15</v>
+      </c>
+      <c r="D67" s="20" t="n">
+        <v>8</v>
+      </c>
+      <c r="E67" s="20" t="n">
+        <v>1</v>
+      </c>
+      <c r="F67" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="G67" s="21"/>
+      <c r="H67" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="I67" s="20" t="s">
+        <v>60</v>
+      </c>
+      <c r="J67" s="20" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -2430,22 +2730,22 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="C18" activeCellId="0" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="21.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="52.32"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="3" style="1" width="10.17"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="4" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -2453,10 +2753,10 @@
     </row>
     <row r="2" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
@@ -2464,10 +2764,10 @@
     </row>
     <row r="3" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>63</v>
+        <v>67</v>
+      </c>
+      <c r="B3" s="23" t="s">
+        <v>68</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>

</xml_diff>

<commit_message>
Pro's Roll Up Week 3
</commit_message>
<xml_diff>
--- a/data/leaguedata.xlsx
+++ b/data/leaguedata.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
     <sheet name="Settings" sheetId="2" state="visible" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" state="visible" r:id="rId5"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="93">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -260,6 +261,21 @@
     <t xml:space="preserve">Jubilee Bowl Stableford – 16 Points</t>
   </si>
   <si>
+    <t xml:space="preserve">Pros Roll Up Week 3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">12.96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1 May 2025</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pros Roll Up Week 3 -Stableford</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.64</t>
+  </si>
+  <si>
     <t xml:space="preserve">Key</t>
   </si>
   <si>
@@ -269,16 +285,76 @@
     <t xml:space="preserve">League Champions Pot</t>
   </si>
   <si>
-    <t xml:space="preserve">52.40</t>
+    <t xml:space="preserve">57.80</t>
   </si>
   <si>
     <t xml:space="preserve">Next Competition</t>
   </si>
   <si>
-    <t xml:space="preserve">Pros Roll Up Week 3 | 01/05/2025</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Monthly Medal | 03/05/2025</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Last Competition</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">2</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="superscript"/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">nd</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Monthly Medal</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">3 May 2025</t>
   </si>
 </sst>
 </file>
@@ -289,7 +365,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -320,7 +396,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFFFF00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
@@ -332,8 +408,15 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <vertAlign val="superscript"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -368,6 +451,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFBF819E"/>
         <bgColor rgb="FF808080"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFA6"/>
+        <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFB66C"/>
+        <bgColor rgb="FFFF99CC"/>
       </patternFill>
     </fill>
   </fills>
@@ -412,13 +507,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="39">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -478,15 +577,27 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -495,6 +606,10 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
@@ -509,16 +624,44 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -567,11 +710,11 @@
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
       <rgbColor rgb="FFCCFFCC"/>
-      <rgbColor rgb="FFFFFF99"/>
+      <rgbColor rgb="FFFFFFA6"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
       <rgbColor rgb="FFCC99FF"/>
-      <rgbColor rgb="FFFFCC99"/>
+      <rgbColor rgb="FFFFB66C"/>
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF99CC00"/>
@@ -770,10 +913,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K81"/>
+  <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I68" activeCellId="0" sqref="I68"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A75" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I89" activeCellId="0" sqref="I89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -783,2418 +926,2935 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="21.24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.61"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="50.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="12.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="50.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="3" width="12.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="13.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="29.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="2" width="29.21"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="14.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="3.59"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="12" style="1" width="10.16"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="3" t="s">
+    <row r="1" s="5" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="4" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="6" t="n">
+      <c r="B2" s="7" t="n">
         <v>62</v>
       </c>
-      <c r="C2" s="7" t="n">
+      <c r="C2" s="8" t="n">
         <v>38</v>
       </c>
-      <c r="D2" s="7" t="n">
+      <c r="D2" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="E2" s="7" t="n">
+      <c r="E2" s="8" t="n">
         <v>17</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="F2" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="8" t="n">
+      <c r="G2" s="9" t="n">
         <v>24.48</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="9" t="s">
+      <c r="J2" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K2" s="6" t="n">
+      <c r="K2" s="7" t="n">
         <v>62</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="6" t="n">
+      <c r="B3" s="7" t="n">
         <v>64</v>
       </c>
-      <c r="C3" s="7" t="n">
+      <c r="C3" s="8" t="n">
         <v>36</v>
       </c>
-      <c r="D3" s="7" t="n">
+      <c r="D3" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="E3" s="7" t="n">
+      <c r="E3" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="F3" s="5" t="s">
+      <c r="F3" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="G3" s="8" t="n">
+      <c r="G3" s="9" t="n">
         <v>16.32</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="9" t="s">
+      <c r="J3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="6" t="n">
+      <c r="K3" s="7" t="n">
         <v>64</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="6" t="n">
+      <c r="B4" s="7" t="n">
         <v>66</v>
       </c>
-      <c r="C4" s="7" t="n">
+      <c r="C4" s="8" t="n">
         <v>35</v>
       </c>
-      <c r="D4" s="7" t="n">
+      <c r="D4" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="E4" s="7" t="n">
+      <c r="E4" s="8" t="n">
         <v>15</v>
       </c>
-      <c r="F4" s="5" t="s">
+      <c r="F4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G4" s="8"/>
-      <c r="H4" s="5" t="s">
+      <c r="G4" s="9"/>
+      <c r="H4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J4" s="9" t="s">
+      <c r="J4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K4" s="6" t="n">
+      <c r="K4" s="7" t="n">
         <v>66</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="B5" s="6" t="n">
+      <c r="B5" s="7" t="n">
         <v>66</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="8" t="n">
         <v>35</v>
       </c>
-      <c r="D5" s="7" t="n">
+      <c r="D5" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="E5" s="7" t="n">
+      <c r="E5" s="8" t="n">
         <v>14</v>
       </c>
-      <c r="F5" s="5" t="s">
+      <c r="F5" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="G5" s="8"/>
-      <c r="H5" s="5" t="s">
+      <c r="G5" s="9"/>
+      <c r="H5" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="9" t="s">
+      <c r="J5" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K5" s="6" t="n">
+      <c r="K5" s="7" t="n">
         <v>66</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" s="6" t="n">
+      <c r="B6" s="7" t="n">
         <v>67</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="8" t="n">
         <v>33</v>
       </c>
-      <c r="D6" s="7" t="n">
+      <c r="D6" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="E6" s="7" t="n">
+      <c r="E6" s="8" t="n">
         <v>13</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="G6" s="8"/>
-      <c r="H6" s="5" t="s">
+      <c r="G6" s="9"/>
+      <c r="H6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J6" s="9" t="s">
+      <c r="J6" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K6" s="6" t="n">
+      <c r="K6" s="7" t="n">
         <v>67</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="6" t="n">
+      <c r="B7" s="7" t="n">
         <v>68</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="8" t="n">
         <v>32</v>
       </c>
-      <c r="D7" s="7" t="n">
+      <c r="D7" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="E7" s="7" t="n">
+      <c r="E7" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="G7" s="8"/>
-      <c r="H7" s="5" t="s">
+      <c r="G7" s="9"/>
+      <c r="H7" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J7" s="9" t="s">
+      <c r="J7" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K7" s="6" t="n">
+      <c r="K7" s="7" t="n">
         <v>68</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="6" t="n">
+      <c r="B8" s="7" t="n">
         <v>71</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C8" s="8" t="n">
         <v>30</v>
       </c>
-      <c r="D8" s="7" t="n">
+      <c r="D8" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="E8" s="7" t="n">
+      <c r="E8" s="8" t="n">
         <v>11</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G8" s="8"/>
-      <c r="H8" s="5" t="s">
+      <c r="G8" s="9"/>
+      <c r="H8" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J8" s="9" t="s">
+      <c r="J8" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K8" s="6" t="n">
+      <c r="K8" s="7" t="n">
         <v>71</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B9" s="6" t="n">
+      <c r="B9" s="7" t="n">
         <v>71</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="8" t="n">
         <v>30</v>
       </c>
-      <c r="D9" s="7" t="n">
+      <c r="D9" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="E9" s="7" t="n">
+      <c r="E9" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G9" s="8"/>
-      <c r="H9" s="5" t="s">
+      <c r="G9" s="9"/>
+      <c r="H9" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J9" s="9" t="s">
+      <c r="J9" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K9" s="6" t="n">
+      <c r="K9" s="7" t="n">
         <v>71</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="5" t="s">
+      <c r="A10" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="6" t="n">
+      <c r="B10" s="7" t="n">
         <v>72</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C10" s="8" t="n">
         <v>30</v>
       </c>
-      <c r="D10" s="7" t="n">
+      <c r="D10" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="E10" s="7" t="n">
+      <c r="E10" s="8" t="n">
         <v>9</v>
       </c>
-      <c r="F10" s="5" t="s">
+      <c r="F10" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="G10" s="8"/>
-      <c r="H10" s="5" t="s">
+      <c r="G10" s="9"/>
+      <c r="H10" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J10" s="9" t="s">
+      <c r="J10" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K10" s="6" t="n">
+      <c r="K10" s="7" t="n">
         <v>72</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B11" s="6" t="n">
+      <c r="B11" s="7" t="n">
         <v>73</v>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C11" s="8" t="n">
         <v>27</v>
       </c>
-      <c r="D11" s="7" t="n">
+      <c r="D11" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="E11" s="7" t="n">
+      <c r="E11" s="8" t="n">
         <v>8</v>
       </c>
-      <c r="F11" s="5" t="s">
+      <c r="F11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="8"/>
-      <c r="H11" s="5" t="s">
+      <c r="G11" s="9"/>
+      <c r="H11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J11" s="9" t="s">
+      <c r="J11" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K11" s="6" t="n">
+      <c r="K11" s="7" t="n">
         <v>73</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="5" t="s">
+      <c r="A12" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="6" t="n">
+      <c r="B12" s="7" t="n">
         <v>73</v>
       </c>
-      <c r="C12" s="7" t="n">
+      <c r="C12" s="8" t="n">
         <v>27</v>
       </c>
-      <c r="D12" s="7" t="n">
+      <c r="D12" s="8" t="n">
         <v>11</v>
       </c>
-      <c r="E12" s="7" t="n">
+      <c r="E12" s="8" t="n">
         <v>7</v>
       </c>
-      <c r="F12" s="5" t="s">
+      <c r="F12" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G12" s="8"/>
-      <c r="H12" s="5" t="s">
+      <c r="G12" s="9"/>
+      <c r="H12" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J12" s="9" t="s">
+      <c r="J12" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K12" s="6" t="n">
+      <c r="K12" s="7" t="n">
         <v>73</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B13" s="6" t="n">
+      <c r="B13" s="7" t="n">
         <v>73</v>
       </c>
-      <c r="C13" s="7" t="n">
+      <c r="C13" s="8" t="n">
         <v>27</v>
       </c>
-      <c r="D13" s="7" t="n">
+      <c r="D13" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="E13" s="7" t="n">
+      <c r="E13" s="8" t="n">
         <v>6</v>
       </c>
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="8"/>
-      <c r="H13" s="5" t="s">
+      <c r="G13" s="9"/>
+      <c r="H13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J13" s="9" t="s">
+      <c r="J13" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K13" s="6" t="n">
+      <c r="K13" s="7" t="n">
         <v>73</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B14" s="6" t="n">
+      <c r="B14" s="7" t="n">
         <v>74</v>
       </c>
-      <c r="C14" s="7" t="n">
+      <c r="C14" s="8" t="n">
         <v>26</v>
       </c>
-      <c r="D14" s="7" t="n">
+      <c r="D14" s="8" t="n">
         <v>13</v>
       </c>
-      <c r="E14" s="7" t="n">
+      <c r="E14" s="8" t="n">
         <v>5</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="G14" s="8"/>
-      <c r="H14" s="5" t="s">
+      <c r="G14" s="9"/>
+      <c r="H14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J14" s="9" t="s">
+      <c r="J14" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K14" s="6" t="n">
+      <c r="K14" s="7" t="n">
         <v>74</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B15" s="6" t="n">
+      <c r="B15" s="7" t="n">
         <v>76</v>
       </c>
-      <c r="C15" s="7" t="n">
+      <c r="C15" s="8" t="n">
         <v>24</v>
       </c>
-      <c r="D15" s="7" t="n">
+      <c r="D15" s="8" t="n">
         <v>14</v>
       </c>
-      <c r="E15" s="7" t="n">
+      <c r="E15" s="8" t="n">
         <v>4</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="G15" s="8"/>
-      <c r="H15" s="5" t="s">
+      <c r="G15" s="9"/>
+      <c r="H15" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J15" s="9" t="s">
+      <c r="J15" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K15" s="6" t="n">
+      <c r="K15" s="7" t="n">
         <v>76</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="5" t="s">
+      <c r="A16" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B16" s="6" t="n">
+      <c r="B16" s="7" t="n">
         <v>77</v>
       </c>
-      <c r="C16" s="7" t="n">
+      <c r="C16" s="8" t="n">
         <v>23</v>
       </c>
-      <c r="D16" s="7" t="n">
+      <c r="D16" s="8" t="n">
         <v>15</v>
       </c>
-      <c r="E16" s="7" t="n">
+      <c r="E16" s="8" t="n">
         <v>3</v>
       </c>
-      <c r="F16" s="5" t="s">
+      <c r="F16" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="G16" s="8"/>
-      <c r="H16" s="5" t="s">
+      <c r="G16" s="9"/>
+      <c r="H16" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I16" s="5" t="s">
+      <c r="I16" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J16" s="9" t="s">
+      <c r="J16" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K16" s="6" t="n">
+      <c r="K16" s="7" t="n">
         <v>77</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B17" s="6" t="n">
+      <c r="B17" s="7" t="n">
         <v>80</v>
       </c>
-      <c r="C17" s="7" t="n">
+      <c r="C17" s="8" t="n">
         <v>21</v>
       </c>
-      <c r="D17" s="7" t="n">
+      <c r="D17" s="8" t="n">
         <v>16</v>
       </c>
-      <c r="E17" s="7" t="n">
+      <c r="E17" s="8" t="n">
         <v>2</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="5" t="s">
+      <c r="G17" s="9"/>
+      <c r="H17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J17" s="9" t="s">
+      <c r="J17" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K17" s="6" t="n">
+      <c r="K17" s="7" t="n">
         <v>80</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="6" t="n">
+      <c r="B18" s="7" t="n">
         <v>91</v>
       </c>
-      <c r="C18" s="7" t="n">
+      <c r="C18" s="8" t="n">
         <v>10</v>
       </c>
-      <c r="D18" s="7" t="n">
+      <c r="D18" s="8" t="n">
         <v>17</v>
       </c>
-      <c r="E18" s="7" t="n">
+      <c r="E18" s="8" t="n">
         <v>1</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="F18" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="G18" s="8"/>
-      <c r="H18" s="5" t="s">
+      <c r="G18" s="9"/>
+      <c r="H18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="J18" s="9" t="s">
+      <c r="J18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K18" s="6" t="n">
+      <c r="K18" s="7" t="n">
         <v>91</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B19" s="11" t="n">
+      <c r="B19" s="12" t="n">
         <v>59</v>
       </c>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11" t="n">
+      <c r="C19" s="12"/>
+      <c r="D19" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="E19" s="11" t="n">
+      <c r="E19" s="12" t="n">
         <v>21</v>
       </c>
-      <c r="F19" s="10" t="s">
+      <c r="F19" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="12" t="n">
+      <c r="G19" s="13" t="n">
         <v>30.24</v>
       </c>
-      <c r="H19" s="10" t="s">
+      <c r="H19" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I19" s="10" t="s">
+      <c r="I19" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J19" s="13" t="s">
+      <c r="J19" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="10" t="s">
+      <c r="A20" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="B20" s="11" t="n">
+      <c r="B20" s="12" t="n">
         <v>61</v>
       </c>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11" t="n">
+      <c r="C20" s="12"/>
+      <c r="D20" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="E20" s="11" t="n">
+      <c r="E20" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="F20" s="10" t="s">
+      <c r="F20" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G20" s="12" t="n">
+      <c r="G20" s="13" t="n">
         <v>20.16</v>
       </c>
-      <c r="H20" s="10" t="s">
+      <c r="H20" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I20" s="10" t="s">
+      <c r="I20" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="13" t="s">
+      <c r="J20" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="10" t="s">
+      <c r="A21" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B21" s="11" t="n">
+      <c r="B21" s="12" t="n">
         <v>63</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11" t="n">
+      <c r="C21" s="12"/>
+      <c r="D21" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="E21" s="11" t="n">
+      <c r="E21" s="12" t="n">
         <v>19</v>
       </c>
-      <c r="F21" s="10" t="s">
+      <c r="F21" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="12"/>
-      <c r="H21" s="10" t="s">
+      <c r="G21" s="13"/>
+      <c r="H21" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I21" s="10" t="s">
+      <c r="I21" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J21" s="13" t="s">
+      <c r="J21" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="10" t="s">
+      <c r="A22" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="B22" s="11" t="n">
+      <c r="B22" s="12" t="n">
         <v>63</v>
       </c>
-      <c r="C22" s="11"/>
-      <c r="D22" s="11" t="n">
+      <c r="C22" s="12"/>
+      <c r="D22" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="E22" s="11" t="n">
+      <c r="E22" s="12" t="n">
         <v>18</v>
       </c>
-      <c r="F22" s="10" t="s">
+      <c r="F22" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G22" s="12"/>
-      <c r="H22" s="10" t="s">
+      <c r="G22" s="13"/>
+      <c r="H22" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I22" s="10" t="s">
+      <c r="I22" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J22" s="13" t="s">
+      <c r="J22" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="10" t="s">
+      <c r="A23" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="B23" s="11" t="n">
+      <c r="B23" s="12" t="n">
         <v>64</v>
       </c>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11" t="n">
+      <c r="C23" s="12"/>
+      <c r="D23" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="E23" s="11" t="n">
+      <c r="E23" s="12" t="n">
         <v>17</v>
       </c>
-      <c r="F23" s="10" t="s">
+      <c r="F23" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="12"/>
-      <c r="H23" s="10" t="s">
+      <c r="G23" s="13"/>
+      <c r="H23" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I23" s="10" t="s">
+      <c r="I23" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J23" s="13" t="s">
+      <c r="J23" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="10" t="s">
+      <c r="A24" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="B24" s="11" t="n">
+      <c r="B24" s="12" t="n">
         <v>64</v>
       </c>
-      <c r="C24" s="11"/>
-      <c r="D24" s="11" t="n">
+      <c r="C24" s="12"/>
+      <c r="D24" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="E24" s="11" t="n">
+      <c r="E24" s="12" t="n">
         <v>16</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="F24" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G24" s="12"/>
-      <c r="H24" s="10" t="s">
+      <c r="G24" s="13"/>
+      <c r="H24" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I24" s="10" t="s">
+      <c r="I24" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J24" s="13" t="s">
+      <c r="J24" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="10" t="s">
+      <c r="A25" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="B25" s="11" t="n">
+      <c r="B25" s="12" t="n">
         <v>65</v>
       </c>
-      <c r="C25" s="11"/>
-      <c r="D25" s="11" t="n">
+      <c r="C25" s="12"/>
+      <c r="D25" s="12" t="n">
         <v>7</v>
       </c>
-      <c r="E25" s="11" t="n">
+      <c r="E25" s="12" t="n">
         <v>15</v>
       </c>
-      <c r="F25" s="10" t="s">
+      <c r="F25" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G25" s="12"/>
-      <c r="H25" s="10" t="s">
+      <c r="G25" s="13"/>
+      <c r="H25" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I25" s="10" t="s">
+      <c r="I25" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J25" s="13" t="s">
+      <c r="J25" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="10" t="s">
+      <c r="A26" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="B26" s="11" t="n">
+      <c r="B26" s="12" t="n">
         <v>65</v>
       </c>
-      <c r="C26" s="11"/>
-      <c r="D26" s="11" t="n">
+      <c r="C26" s="12"/>
+      <c r="D26" s="12" t="n">
         <v>8</v>
       </c>
-      <c r="E26" s="11" t="n">
+      <c r="E26" s="12" t="n">
         <v>14</v>
       </c>
-      <c r="F26" s="10" t="s">
+      <c r="F26" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G26" s="12"/>
-      <c r="H26" s="10" t="s">
+      <c r="G26" s="13"/>
+      <c r="H26" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I26" s="10" t="s">
+      <c r="I26" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J26" s="13" t="s">
+      <c r="J26" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="10" t="s">
+      <c r="A27" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="B27" s="11" t="n">
+      <c r="B27" s="12" t="n">
         <v>66</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11" t="n">
+      <c r="C27" s="12"/>
+      <c r="D27" s="12" t="n">
         <v>9</v>
       </c>
-      <c r="E27" s="11" t="n">
+      <c r="E27" s="12" t="n">
         <v>13</v>
       </c>
-      <c r="F27" s="10" t="s">
+      <c r="F27" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G27" s="12"/>
-      <c r="H27" s="10" t="s">
+      <c r="G27" s="13"/>
+      <c r="H27" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I27" s="10" t="s">
+      <c r="I27" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J27" s="13" t="s">
+      <c r="J27" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="10" t="s">
+      <c r="A28" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B28" s="11" t="n">
+      <c r="B28" s="12" t="n">
         <v>68</v>
       </c>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11" t="n">
+      <c r="C28" s="12"/>
+      <c r="D28" s="12" t="n">
         <v>10</v>
       </c>
-      <c r="E28" s="11" t="n">
+      <c r="E28" s="12" t="n">
         <v>12</v>
       </c>
-      <c r="F28" s="10" t="s">
+      <c r="F28" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G28" s="12"/>
-      <c r="H28" s="10" t="s">
+      <c r="G28" s="13"/>
+      <c r="H28" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I28" s="10" t="s">
+      <c r="I28" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J28" s="13" t="s">
+      <c r="J28" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="11" t="n">
+      <c r="B29" s="12" t="n">
         <v>69</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="11" t="n">
+      <c r="C29" s="12"/>
+      <c r="D29" s="12" t="n">
         <v>11</v>
       </c>
-      <c r="E29" s="11" t="n">
+      <c r="E29" s="12" t="n">
         <v>11</v>
       </c>
-      <c r="F29" s="10" t="s">
+      <c r="F29" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G29" s="12"/>
-      <c r="H29" s="10" t="s">
+      <c r="G29" s="13"/>
+      <c r="H29" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I29" s="10" t="s">
+      <c r="I29" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J29" s="13" t="s">
+      <c r="J29" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="10" t="s">
+      <c r="A30" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="11" t="n">
+      <c r="B30" s="12" t="n">
         <v>70</v>
       </c>
-      <c r="C30" s="11"/>
-      <c r="D30" s="11" t="n">
+      <c r="C30" s="12"/>
+      <c r="D30" s="12" t="n">
         <v>12</v>
       </c>
-      <c r="E30" s="11" t="n">
+      <c r="E30" s="12" t="n">
         <v>10</v>
       </c>
-      <c r="F30" s="10" t="s">
+      <c r="F30" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G30" s="12"/>
-      <c r="H30" s="10" t="s">
+      <c r="G30" s="13"/>
+      <c r="H30" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I30" s="10" t="s">
+      <c r="I30" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J30" s="13" t="s">
+      <c r="J30" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="10" t="s">
+      <c r="A31" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="11" t="n">
+      <c r="B31" s="12" t="n">
         <v>70</v>
       </c>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11" t="n">
+      <c r="C31" s="12"/>
+      <c r="D31" s="12" t="n">
         <v>13</v>
       </c>
-      <c r="E31" s="11" t="n">
+      <c r="E31" s="12" t="n">
         <v>9</v>
       </c>
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G31" s="12"/>
-      <c r="H31" s="10" t="s">
+      <c r="G31" s="13"/>
+      <c r="H31" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I31" s="10" t="s">
+      <c r="I31" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J31" s="13" t="s">
+      <c r="J31" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="10" t="s">
+      <c r="A32" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="B32" s="11" t="n">
+      <c r="B32" s="12" t="n">
         <v>71</v>
       </c>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11" t="n">
+      <c r="C32" s="12"/>
+      <c r="D32" s="12" t="n">
         <v>14</v>
       </c>
-      <c r="E32" s="11" t="n">
+      <c r="E32" s="12" t="n">
         <v>8</v>
       </c>
-      <c r="F32" s="10" t="s">
+      <c r="F32" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G32" s="12"/>
-      <c r="H32" s="10" t="s">
+      <c r="G32" s="13"/>
+      <c r="H32" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I32" s="10" t="s">
+      <c r="I32" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J32" s="13" t="s">
+      <c r="J32" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="10" t="s">
+      <c r="A33" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="B33" s="11" t="n">
+      <c r="B33" s="12" t="n">
         <v>72</v>
       </c>
-      <c r="C33" s="11"/>
-      <c r="D33" s="11" t="n">
+      <c r="C33" s="12"/>
+      <c r="D33" s="12" t="n">
         <v>15</v>
       </c>
-      <c r="E33" s="11" t="n">
+      <c r="E33" s="12" t="n">
         <v>7</v>
       </c>
-      <c r="F33" s="10" t="s">
+      <c r="F33" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G33" s="12"/>
-      <c r="H33" s="10" t="s">
+      <c r="G33" s="13"/>
+      <c r="H33" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I33" s="10" t="s">
+      <c r="I33" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J33" s="13" t="s">
+      <c r="J33" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="10" t="s">
+      <c r="A34" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="B34" s="11" t="n">
+      <c r="B34" s="12" t="n">
         <v>72</v>
       </c>
-      <c r="C34" s="11"/>
-      <c r="D34" s="11" t="n">
+      <c r="C34" s="12"/>
+      <c r="D34" s="12" t="n">
         <v>16</v>
       </c>
-      <c r="E34" s="11" t="n">
+      <c r="E34" s="12" t="n">
         <v>6</v>
       </c>
-      <c r="F34" s="10" t="s">
+      <c r="F34" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G34" s="12"/>
-      <c r="H34" s="10" t="s">
+      <c r="G34" s="13"/>
+      <c r="H34" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I34" s="10" t="s">
+      <c r="I34" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J34" s="13" t="s">
+      <c r="J34" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="10" t="s">
+      <c r="A35" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="B35" s="11" t="n">
+      <c r="B35" s="12" t="n">
         <v>73</v>
       </c>
-      <c r="C35" s="11"/>
-      <c r="D35" s="11" t="n">
+      <c r="C35" s="12"/>
+      <c r="D35" s="12" t="n">
         <v>17</v>
       </c>
-      <c r="E35" s="11" t="n">
+      <c r="E35" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="F35" s="10" t="s">
+      <c r="F35" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G35" s="12"/>
-      <c r="H35" s="10" t="s">
+      <c r="G35" s="13"/>
+      <c r="H35" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I35" s="10" t="s">
+      <c r="I35" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J35" s="13" t="s">
+      <c r="J35" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="10" t="s">
+      <c r="A36" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="B36" s="11" t="n">
+      <c r="B36" s="12" t="n">
         <v>76</v>
       </c>
-      <c r="C36" s="11"/>
-      <c r="D36" s="11" t="n">
+      <c r="C36" s="12"/>
+      <c r="D36" s="12" t="n">
         <v>18</v>
       </c>
-      <c r="E36" s="11" t="n">
+      <c r="E36" s="12" t="n">
         <v>4</v>
       </c>
-      <c r="F36" s="10" t="s">
+      <c r="F36" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G36" s="12"/>
-      <c r="H36" s="10" t="s">
+      <c r="G36" s="13"/>
+      <c r="H36" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I36" s="10" t="s">
+      <c r="I36" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J36" s="13" t="s">
+      <c r="J36" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="10" t="s">
+      <c r="A37" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B37" s="11" t="n">
+      <c r="B37" s="12" t="n">
         <v>77</v>
       </c>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11" t="n">
+      <c r="C37" s="12"/>
+      <c r="D37" s="12" t="n">
         <v>19</v>
       </c>
-      <c r="E37" s="11" t="n">
+      <c r="E37" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="F37" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G37" s="12"/>
-      <c r="H37" s="10" t="s">
+      <c r="G37" s="13"/>
+      <c r="H37" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I37" s="10" t="s">
+      <c r="I37" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J37" s="13" t="s">
+      <c r="J37" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="10" t="s">
+      <c r="A38" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="11" t="n">
+      <c r="B38" s="12" t="n">
         <v>77</v>
       </c>
-      <c r="C38" s="11"/>
-      <c r="D38" s="11" t="n">
+      <c r="C38" s="12"/>
+      <c r="D38" s="12" t="n">
         <v>20</v>
       </c>
-      <c r="E38" s="11" t="n">
+      <c r="E38" s="12" t="n">
         <v>2</v>
       </c>
-      <c r="F38" s="10" t="s">
+      <c r="F38" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G38" s="12"/>
-      <c r="H38" s="10" t="s">
+      <c r="G38" s="13"/>
+      <c r="H38" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I38" s="10" t="s">
+      <c r="I38" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J38" s="13" t="s">
+      <c r="J38" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="10" t="s">
+      <c r="A39" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="11" t="n">
+      <c r="B39" s="12" t="n">
         <v>80</v>
       </c>
-      <c r="C39" s="11"/>
-      <c r="D39" s="11" t="n">
+      <c r="C39" s="12"/>
+      <c r="D39" s="12" t="n">
         <v>21</v>
       </c>
-      <c r="E39" s="11" t="n">
+      <c r="E39" s="12" t="n">
         <v>1</v>
       </c>
-      <c r="F39" s="10" t="s">
+      <c r="F39" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G39" s="12"/>
-      <c r="H39" s="10" t="s">
+      <c r="G39" s="13"/>
+      <c r="H39" s="11" t="s">
         <v>44</v>
       </c>
-      <c r="I39" s="10" t="s">
+      <c r="I39" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="J39" s="13" t="s">
+      <c r="J39" s="14" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="14" t="s">
+      <c r="A40" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="B40" s="15" t="n">
+      <c r="B40" s="16" t="n">
         <v>60</v>
       </c>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15" t="n">
+      <c r="C40" s="16"/>
+      <c r="D40" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="E40" s="15" t="n">
+      <c r="E40" s="16" t="n">
         <v>20</v>
       </c>
-      <c r="F40" s="16" t="s">
+      <c r="F40" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G40" s="17" t="s">
+      <c r="G40" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="H40" s="15" t="s">
+      <c r="H40" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I40" s="16" t="s">
+      <c r="I40" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="J40" s="16" t="s">
+      <c r="J40" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="14" t="s">
+      <c r="A41" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="B41" s="15" t="n">
+      <c r="B41" s="16" t="n">
         <v>63</v>
       </c>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15" t="n">
+      <c r="C41" s="16"/>
+      <c r="D41" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="E41" s="15" t="n">
+      <c r="E41" s="16" t="n">
         <v>19</v>
       </c>
-      <c r="F41" s="16" t="s">
+      <c r="F41" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G41" s="17" t="s">
+      <c r="G41" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="H41" s="15" t="s">
+      <c r="H41" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I41" s="15" t="s">
+      <c r="I41" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J41" s="16" t="s">
+      <c r="J41" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="14" t="s">
+      <c r="A42" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="B42" s="15" t="n">
+      <c r="B42" s="16" t="n">
         <v>63</v>
       </c>
-      <c r="C42" s="15"/>
-      <c r="D42" s="15" t="n">
+      <c r="C42" s="16"/>
+      <c r="D42" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="E42" s="15" t="n">
+      <c r="E42" s="16" t="n">
         <v>18</v>
       </c>
-      <c r="F42" s="16" t="s">
+      <c r="F42" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G42" s="17"/>
-      <c r="H42" s="15" t="s">
+      <c r="G42" s="18"/>
+      <c r="H42" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I42" s="15" t="s">
+      <c r="I42" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J42" s="16" t="s">
+      <c r="J42" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="14" t="s">
+      <c r="A43" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="15" t="n">
+      <c r="B43" s="16" t="n">
         <v>64</v>
       </c>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15" t="n">
+      <c r="C43" s="16"/>
+      <c r="D43" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="E43" s="15" t="n">
+      <c r="E43" s="16" t="n">
         <v>17</v>
       </c>
-      <c r="F43" s="16" t="s">
+      <c r="F43" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G43" s="17"/>
-      <c r="H43" s="15" t="s">
+      <c r="G43" s="18"/>
+      <c r="H43" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I43" s="15" t="s">
+      <c r="I43" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J43" s="16" t="s">
+      <c r="J43" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="B44" s="15" t="n">
+      <c r="B44" s="16" t="n">
         <v>65</v>
       </c>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15" t="n">
+      <c r="C44" s="16"/>
+      <c r="D44" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="E44" s="15" t="n">
+      <c r="E44" s="16" t="n">
         <v>16</v>
       </c>
-      <c r="F44" s="16" t="s">
+      <c r="F44" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G44" s="17"/>
-      <c r="H44" s="15" t="s">
+      <c r="G44" s="18"/>
+      <c r="H44" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I44" s="15" t="s">
+      <c r="I44" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J44" s="16" t="s">
+      <c r="J44" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="14" t="s">
+      <c r="A45" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="B45" s="15" t="n">
+      <c r="B45" s="16" t="n">
         <v>66</v>
       </c>
-      <c r="C45" s="15"/>
-      <c r="D45" s="15" t="n">
+      <c r="C45" s="16"/>
+      <c r="D45" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="E45" s="15" t="n">
+      <c r="E45" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="F45" s="16" t="s">
+      <c r="F45" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G45" s="17"/>
-      <c r="H45" s="15" t="s">
+      <c r="G45" s="18"/>
+      <c r="H45" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I45" s="15" t="s">
+      <c r="I45" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J45" s="16" t="s">
+      <c r="J45" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="14" t="s">
+      <c r="A46" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B46" s="15" t="n">
+      <c r="B46" s="16" t="n">
         <v>67</v>
       </c>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15" t="n">
+      <c r="C46" s="16"/>
+      <c r="D46" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="E46" s="15" t="n">
+      <c r="E46" s="16" t="n">
         <v>14</v>
       </c>
-      <c r="F46" s="16" t="s">
+      <c r="F46" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G46" s="17"/>
-      <c r="H46" s="15" t="s">
+      <c r="G46" s="18"/>
+      <c r="H46" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I46" s="15" t="s">
+      <c r="I46" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J46" s="16" t="s">
+      <c r="J46" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="14" t="s">
+      <c r="A47" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B47" s="15" t="n">
+      <c r="B47" s="16" t="n">
         <v>67</v>
       </c>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15" t="n">
+      <c r="C47" s="16"/>
+      <c r="D47" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="E47" s="15" t="n">
+      <c r="E47" s="16" t="n">
         <v>13</v>
       </c>
-      <c r="F47" s="16" t="s">
+      <c r="F47" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G47" s="17"/>
-      <c r="H47" s="15" t="s">
+      <c r="G47" s="18"/>
+      <c r="H47" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I47" s="15" t="s">
+      <c r="I47" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J47" s="16" t="s">
+      <c r="J47" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="14" t="s">
+      <c r="A48" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B48" s="15" t="n">
+      <c r="B48" s="16" t="n">
         <v>68</v>
       </c>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15" t="n">
+      <c r="C48" s="16"/>
+      <c r="D48" s="16" t="n">
         <v>9</v>
       </c>
-      <c r="E48" s="15" t="n">
+      <c r="E48" s="16" t="n">
         <v>12</v>
       </c>
-      <c r="F48" s="16" t="s">
+      <c r="F48" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G48" s="17"/>
-      <c r="H48" s="15" t="s">
+      <c r="G48" s="18"/>
+      <c r="H48" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I48" s="15" t="s">
+      <c r="I48" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J48" s="16" t="s">
+      <c r="J48" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="15" t="s">
+      <c r="A49" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="B49" s="15" t="n">
+      <c r="B49" s="16" t="n">
         <v>68</v>
       </c>
-      <c r="C49" s="15"/>
-      <c r="D49" s="15" t="n">
+      <c r="C49" s="16"/>
+      <c r="D49" s="16" t="n">
         <v>10</v>
       </c>
-      <c r="E49" s="15" t="n">
+      <c r="E49" s="16" t="n">
         <v>11</v>
       </c>
-      <c r="F49" s="16" t="s">
+      <c r="F49" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G49" s="17"/>
-      <c r="H49" s="15" t="s">
+      <c r="G49" s="18"/>
+      <c r="H49" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I49" s="15" t="s">
+      <c r="I49" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J49" s="16" t="s">
+      <c r="J49" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="B50" s="15" t="n">
+      <c r="B50" s="16" t="n">
         <v>69</v>
       </c>
-      <c r="C50" s="15"/>
-      <c r="D50" s="15" t="n">
+      <c r="C50" s="16"/>
+      <c r="D50" s="16" t="n">
         <v>11</v>
       </c>
-      <c r="E50" s="15" t="n">
+      <c r="E50" s="16" t="n">
         <v>10</v>
       </c>
-      <c r="F50" s="16" t="s">
+      <c r="F50" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G50" s="17"/>
-      <c r="H50" s="15" t="s">
+      <c r="G50" s="18"/>
+      <c r="H50" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I50" s="15" t="s">
+      <c r="I50" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J50" s="16" t="s">
+      <c r="J50" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="15" t="s">
+      <c r="A51" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="B51" s="15" t="n">
+      <c r="B51" s="16" t="n">
         <v>71</v>
       </c>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15" t="n">
+      <c r="C51" s="16"/>
+      <c r="D51" s="16" t="n">
         <v>12</v>
       </c>
-      <c r="E51" s="15" t="n">
+      <c r="E51" s="16" t="n">
         <v>9</v>
       </c>
-      <c r="F51" s="16" t="s">
+      <c r="F51" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G51" s="17"/>
-      <c r="H51" s="15" t="s">
+      <c r="G51" s="18"/>
+      <c r="H51" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I51" s="15" t="s">
+      <c r="I51" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J51" s="16" t="s">
+      <c r="J51" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="15" t="s">
+      <c r="A52" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="B52" s="15" t="n">
+      <c r="B52" s="16" t="n">
         <v>71</v>
       </c>
-      <c r="C52" s="15"/>
-      <c r="D52" s="15" t="n">
+      <c r="C52" s="16"/>
+      <c r="D52" s="16" t="n">
         <v>13</v>
       </c>
-      <c r="E52" s="15" t="n">
+      <c r="E52" s="16" t="n">
         <v>8</v>
       </c>
-      <c r="F52" s="16" t="s">
+      <c r="F52" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G52" s="17"/>
-      <c r="H52" s="15" t="s">
+      <c r="G52" s="18"/>
+      <c r="H52" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I52" s="15" t="s">
+      <c r="I52" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J52" s="16" t="s">
+      <c r="J52" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="15" t="s">
+      <c r="A53" s="16" t="s">
         <v>28</v>
       </c>
-      <c r="B53" s="15" t="n">
+      <c r="B53" s="16" t="n">
         <v>72</v>
       </c>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15" t="n">
+      <c r="C53" s="16"/>
+      <c r="D53" s="16" t="n">
         <v>14</v>
       </c>
-      <c r="E53" s="15" t="n">
+      <c r="E53" s="16" t="n">
         <v>7</v>
       </c>
-      <c r="F53" s="16" t="s">
+      <c r="F53" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G53" s="17"/>
-      <c r="H53" s="15" t="s">
+      <c r="G53" s="18"/>
+      <c r="H53" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I53" s="15" t="s">
+      <c r="I53" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J53" s="16" t="s">
+      <c r="J53" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="16" t="s">
         <v>27</v>
       </c>
-      <c r="B54" s="15" t="n">
+      <c r="B54" s="16" t="n">
         <v>72</v>
       </c>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15" t="n">
+      <c r="C54" s="16"/>
+      <c r="D54" s="16" t="n">
         <v>15</v>
       </c>
-      <c r="E54" s="15" t="n">
+      <c r="E54" s="16" t="n">
         <v>6</v>
       </c>
-      <c r="F54" s="16" t="s">
+      <c r="F54" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G54" s="17"/>
-      <c r="H54" s="15" t="s">
+      <c r="G54" s="18"/>
+      <c r="H54" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I54" s="15" t="s">
+      <c r="I54" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J54" s="16" t="s">
+      <c r="J54" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="15" t="s">
+      <c r="A55" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B55" s="15" t="n">
+      <c r="B55" s="16" t="n">
         <v>72</v>
       </c>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15" t="n">
+      <c r="C55" s="16"/>
+      <c r="D55" s="16" t="n">
         <v>16</v>
       </c>
-      <c r="E55" s="15" t="n">
+      <c r="E55" s="16" t="n">
         <v>5</v>
       </c>
-      <c r="F55" s="16" t="s">
+      <c r="F55" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G55" s="17"/>
-      <c r="H55" s="15" t="s">
+      <c r="G55" s="18"/>
+      <c r="H55" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I55" s="15" t="s">
+      <c r="I55" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J55" s="16" t="s">
+      <c r="J55" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="15" t="s">
+      <c r="A56" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="B56" s="15" t="n">
+      <c r="B56" s="16" t="n">
         <v>75</v>
       </c>
-      <c r="C56" s="15"/>
-      <c r="D56" s="15" t="n">
+      <c r="C56" s="16"/>
+      <c r="D56" s="16" t="n">
         <v>17</v>
       </c>
-      <c r="E56" s="15" t="n">
+      <c r="E56" s="16" t="n">
         <v>4</v>
       </c>
-      <c r="F56" s="16" t="s">
+      <c r="F56" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G56" s="17"/>
-      <c r="H56" s="15" t="s">
+      <c r="G56" s="18"/>
+      <c r="H56" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I56" s="15" t="s">
+      <c r="I56" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J56" s="16" t="s">
+      <c r="J56" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="15" t="s">
+      <c r="A57" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="B57" s="15" t="n">
+      <c r="B57" s="16" t="n">
         <v>76</v>
       </c>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15" t="n">
+      <c r="C57" s="16"/>
+      <c r="D57" s="16" t="n">
         <v>18</v>
       </c>
-      <c r="E57" s="15" t="n">
+      <c r="E57" s="16" t="n">
         <v>3</v>
       </c>
-      <c r="F57" s="16" t="s">
+      <c r="F57" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G57" s="17"/>
-      <c r="H57" s="15" t="s">
+      <c r="G57" s="18"/>
+      <c r="H57" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I57" s="15" t="s">
+      <c r="I57" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J57" s="16" t="s">
+      <c r="J57" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="15" t="s">
+      <c r="A58" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="B58" s="15" t="n">
+      <c r="B58" s="16" t="n">
         <v>86</v>
       </c>
-      <c r="C58" s="15"/>
-      <c r="D58" s="15" t="n">
+      <c r="C58" s="16"/>
+      <c r="D58" s="16" t="n">
         <v>19</v>
       </c>
-      <c r="E58" s="15" t="n">
+      <c r="E58" s="16" t="n">
         <v>2</v>
       </c>
-      <c r="F58" s="16" t="s">
+      <c r="F58" s="17" t="s">
         <v>51</v>
       </c>
-      <c r="G58" s="17"/>
-      <c r="H58" s="15" t="s">
+      <c r="G58" s="18"/>
+      <c r="H58" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I58" s="15" t="s">
+      <c r="I58" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J58" s="16" t="s">
+      <c r="J58" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="15" t="s">
+      <c r="A59" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="B59" s="15" t="n">
+      <c r="B59" s="16" t="n">
         <v>0</v>
       </c>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15" t="n">
+      <c r="C59" s="16"/>
+      <c r="D59" s="16" t="n">
         <v>20</v>
       </c>
-      <c r="E59" s="15" t="n">
+      <c r="E59" s="16" t="n">
         <v>1</v>
       </c>
-      <c r="F59" s="16" t="s">
+      <c r="F59" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="G59" s="17"/>
-      <c r="H59" s="15" t="s">
+      <c r="G59" s="18"/>
+      <c r="H59" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="I59" s="15" t="s">
+      <c r="I59" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="J59" s="16" t="s">
+      <c r="J59" s="19" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="18" t="s">
+      <c r="A60" s="21" t="s">
         <v>22</v>
       </c>
-      <c r="B60" s="18" t="n">
+      <c r="B60" s="21" t="n">
         <v>38</v>
       </c>
-      <c r="C60" s="18" t="n">
+      <c r="C60" s="21" t="n">
         <v>19</v>
       </c>
-      <c r="D60" s="18" t="n">
+      <c r="D60" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="E60" s="18" t="n">
+      <c r="E60" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="F60" s="18" t="s">
+      <c r="F60" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G60" s="19" t="s">
+      <c r="G60" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="H60" s="18" t="s">
+      <c r="H60" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="I60" s="18" t="s">
+      <c r="I60" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="J60" s="18" t="s">
+      <c r="J60" s="21" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="18" t="s">
+      <c r="A61" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="B61" s="18" t="n">
+      <c r="B61" s="21" t="n">
         <v>39</v>
       </c>
-      <c r="C61" s="18" t="n">
+      <c r="C61" s="21" t="n">
         <v>18</v>
       </c>
-      <c r="D61" s="18" t="n">
+      <c r="D61" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="E61" s="18" t="n">
+      <c r="E61" s="21" t="n">
         <v>7</v>
       </c>
-      <c r="F61" s="18" t="s">
+      <c r="F61" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G61" s="19" t="s">
+      <c r="G61" s="23" t="s">
         <v>62</v>
       </c>
-      <c r="H61" s="18" t="s">
+      <c r="H61" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="I61" s="18" t="s">
+      <c r="I61" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="J61" s="18" t="s">
+      <c r="J61" s="21" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="18" t="s">
+      <c r="A62" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="B62" s="18" t="n">
+      <c r="B62" s="21" t="n">
         <v>39</v>
       </c>
-      <c r="C62" s="18" t="n">
+      <c r="C62" s="21" t="n">
         <v>18</v>
       </c>
-      <c r="D62" s="18" t="n">
+      <c r="D62" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="E62" s="18" t="n">
+      <c r="E62" s="21" t="n">
         <v>6</v>
       </c>
-      <c r="F62" s="18" t="s">
+      <c r="F62" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G62" s="19"/>
-      <c r="H62" s="18" t="s">
+      <c r="G62" s="23"/>
+      <c r="H62" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="I62" s="18" t="s">
+      <c r="I62" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="J62" s="18" t="s">
+      <c r="J62" s="21" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="18" t="s">
+      <c r="A63" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="B63" s="18" t="n">
+      <c r="B63" s="21" t="n">
         <v>42</v>
       </c>
-      <c r="C63" s="18" t="n">
+      <c r="C63" s="21" t="n">
         <v>17</v>
       </c>
-      <c r="D63" s="18" t="n">
+      <c r="D63" s="21" t="n">
         <v>4</v>
       </c>
-      <c r="E63" s="18" t="n">
+      <c r="E63" s="21" t="n">
         <v>5</v>
       </c>
-      <c r="F63" s="18" t="s">
+      <c r="F63" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G63" s="19"/>
-      <c r="H63" s="18" t="s">
+      <c r="G63" s="23"/>
+      <c r="H63" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="I63" s="18" t="s">
+      <c r="I63" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="J63" s="18" t="s">
+      <c r="J63" s="21" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="64" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="20" t="s">
+    <row r="64" s="27" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="24" t="s">
         <v>20</v>
       </c>
-      <c r="B64" s="20" t="n">
+      <c r="B64" s="24" t="n">
         <v>40</v>
       </c>
-      <c r="C64" s="20" t="n">
+      <c r="C64" s="24" t="n">
         <v>17</v>
       </c>
-      <c r="D64" s="20" t="n">
+      <c r="D64" s="24" t="n">
         <v>5</v>
       </c>
-      <c r="E64" s="20" t="n">
+      <c r="E64" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="F64" s="20" t="s">
+      <c r="F64" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="G64" s="21"/>
-      <c r="H64" s="18" t="s">
+      <c r="G64" s="26"/>
+      <c r="H64" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="I64" s="20" t="s">
+      <c r="I64" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="J64" s="20" t="s">
+      <c r="J64" s="24" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="18" t="s">
+      <c r="A65" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="B65" s="18" t="n">
+      <c r="B65" s="21" t="n">
         <v>38</v>
       </c>
-      <c r="C65" s="18" t="n">
+      <c r="C65" s="21" t="n">
         <v>17</v>
       </c>
-      <c r="D65" s="18" t="n">
+      <c r="D65" s="21" t="n">
         <v>6</v>
       </c>
-      <c r="E65" s="18" t="n">
+      <c r="E65" s="21" t="n">
         <v>3</v>
       </c>
-      <c r="F65" s="18" t="s">
+      <c r="F65" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G65" s="19"/>
-      <c r="H65" s="18" t="s">
+      <c r="G65" s="23"/>
+      <c r="H65" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="I65" s="18" t="s">
+      <c r="I65" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="J65" s="18" t="s">
+      <c r="J65" s="21" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="18" t="s">
+      <c r="A66" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="B66" s="18" t="n">
+      <c r="B66" s="21" t="n">
         <v>42</v>
       </c>
-      <c r="C66" s="18" t="n">
+      <c r="C66" s="21" t="n">
         <v>17</v>
       </c>
-      <c r="D66" s="18" t="n">
+      <c r="D66" s="21" t="n">
         <v>7</v>
       </c>
-      <c r="E66" s="18" t="n">
+      <c r="E66" s="21" t="n">
         <v>2</v>
       </c>
-      <c r="F66" s="18" t="s">
+      <c r="F66" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="G66" s="19"/>
-      <c r="H66" s="18" t="s">
+      <c r="G66" s="23"/>
+      <c r="H66" s="21" t="s">
         <v>59</v>
       </c>
-      <c r="I66" s="18" t="s">
+      <c r="I66" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="J66" s="18" t="s">
+      <c r="J66" s="21" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="67" s="22" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="20" t="s">
+    <row r="67" s="27" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="B67" s="20" t="n">
+      <c r="B67" s="24" t="n">
         <v>40</v>
       </c>
-      <c r="C67" s="20" t="n">
+      <c r="C67" s="24" t="n">
         <v>15</v>
       </c>
-      <c r="D67" s="20" t="n">
+      <c r="D67" s="24" t="n">
         <v>8</v>
       </c>
-      <c r="E67" s="20" t="n">
+      <c r="E67" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="F67" s="20" t="s">
+      <c r="F67" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="G67" s="21"/>
-      <c r="H67" s="18" t="s">
+      <c r="G67" s="26"/>
+      <c r="H67" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="I67" s="20" t="s">
+      <c r="I67" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="J67" s="20" t="s">
+      <c r="J67" s="24" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="23" t="s">
+      <c r="A68" s="28" t="s">
         <v>39</v>
       </c>
-      <c r="B68" s="23" t="n">
+      <c r="B68" s="28" t="n">
         <v>62</v>
       </c>
-      <c r="C68" s="23" t="n">
+      <c r="C68" s="28" t="n">
         <v>38</v>
       </c>
-      <c r="D68" s="23" t="n">
+      <c r="D68" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="E68" s="23" t="n">
+      <c r="E68" s="28" t="n">
         <v>13</v>
       </c>
-      <c r="F68" s="23" t="s">
+      <c r="F68" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="G68" s="24" t="s">
+      <c r="G68" s="30" t="s">
         <v>64</v>
       </c>
-      <c r="H68" s="23" t="s">
+      <c r="H68" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="I68" s="23" t="s">
+      <c r="I68" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="J68" s="23" t="s">
+      <c r="J68" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="23" t="s">
+      <c r="A69" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B69" s="23" t="n">
+      <c r="B69" s="28" t="n">
         <v>63</v>
       </c>
-      <c r="C69" s="23" t="n">
+      <c r="C69" s="28" t="n">
         <v>37</v>
       </c>
-      <c r="D69" s="23" t="n">
+      <c r="D69" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="E69" s="23" t="n">
+      <c r="E69" s="28" t="n">
         <v>12</v>
       </c>
-      <c r="F69" s="23" t="s">
+      <c r="F69" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="G69" s="24" t="s">
+      <c r="G69" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="H69" s="23" t="s">
+      <c r="H69" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="I69" s="23" t="s">
+      <c r="I69" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="J69" s="23" t="s">
+      <c r="J69" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="23" t="s">
+      <c r="A70" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="B70" s="23" t="n">
+      <c r="B70" s="28" t="n">
         <v>64</v>
       </c>
-      <c r="C70" s="23" t="n">
+      <c r="C70" s="28" t="n">
         <v>35</v>
       </c>
-      <c r="D70" s="23" t="n">
+      <c r="D70" s="28" t="n">
         <v>3</v>
       </c>
-      <c r="E70" s="23" t="n">
+      <c r="E70" s="28" t="n">
         <v>11</v>
       </c>
-      <c r="F70" s="23" t="s">
+      <c r="F70" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="G70" s="24"/>
-      <c r="H70" s="23" t="s">
+      <c r="G70" s="30"/>
+      <c r="H70" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="I70" s="23" t="s">
+      <c r="I70" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="J70" s="23" t="s">
+      <c r="J70" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="23" t="s">
+      <c r="A71" s="28" t="s">
         <v>35</v>
       </c>
-      <c r="B71" s="23" t="n">
+      <c r="B71" s="28" t="n">
         <v>66</v>
       </c>
-      <c r="C71" s="23" t="n">
+      <c r="C71" s="28" t="n">
         <v>34</v>
       </c>
-      <c r="D71" s="23" t="n">
+      <c r="D71" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="E71" s="23" t="n">
+      <c r="E71" s="28" t="n">
         <v>10</v>
       </c>
-      <c r="F71" s="23" t="s">
+      <c r="F71" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="G71" s="24"/>
-      <c r="H71" s="23" t="s">
+      <c r="G71" s="30"/>
+      <c r="H71" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="I71" s="23" t="s">
+      <c r="I71" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="J71" s="23" t="s">
+      <c r="J71" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="23" t="s">
+      <c r="A72" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="B72" s="23" t="n">
+      <c r="B72" s="28" t="n">
         <v>66</v>
       </c>
-      <c r="C72" s="23" t="n">
+      <c r="C72" s="28" t="n">
         <v>33</v>
       </c>
-      <c r="D72" s="23" t="n">
+      <c r="D72" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="E72" s="23" t="n">
+      <c r="E72" s="28" t="n">
         <v>9</v>
       </c>
-      <c r="F72" s="23" t="s">
+      <c r="F72" s="29" t="s">
         <v>71</v>
       </c>
-      <c r="G72" s="24"/>
-      <c r="H72" s="23" t="s">
+      <c r="G72" s="30"/>
+      <c r="H72" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="I72" s="23" t="s">
+      <c r="I72" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="J72" s="23" t="s">
+      <c r="J72" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="23" t="s">
+      <c r="A73" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="B73" s="23" t="n">
+      <c r="B73" s="28" t="n">
         <v>68</v>
       </c>
-      <c r="C73" s="23" t="n">
+      <c r="C73" s="28" t="n">
         <v>32</v>
       </c>
-      <c r="D73" s="23" t="n">
+      <c r="D73" s="28" t="n">
         <v>6</v>
       </c>
-      <c r="E73" s="23" t="n">
+      <c r="E73" s="28" t="n">
         <v>8</v>
       </c>
-      <c r="F73" s="23" t="s">
+      <c r="F73" s="29" t="s">
         <v>72</v>
       </c>
-      <c r="G73" s="24"/>
-      <c r="H73" s="23" t="s">
+      <c r="G73" s="30"/>
+      <c r="H73" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="I73" s="23" t="s">
+      <c r="I73" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="J73" s="23" t="s">
+      <c r="J73" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="23" t="s">
+      <c r="A74" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="B74" s="23" t="n">
+      <c r="B74" s="28" t="n">
         <v>69</v>
       </c>
-      <c r="C74" s="23" t="n">
+      <c r="C74" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="D74" s="23" t="n">
+      <c r="D74" s="28" t="n">
         <v>7</v>
       </c>
-      <c r="E74" s="23" t="n">
+      <c r="E74" s="28" t="n">
         <v>7</v>
       </c>
-      <c r="F74" s="23" t="s">
+      <c r="F74" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="G74" s="24"/>
-      <c r="H74" s="23" t="s">
+      <c r="G74" s="30"/>
+      <c r="H74" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="I74" s="23" t="s">
+      <c r="I74" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="J74" s="23" t="s">
+      <c r="J74" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="23" t="s">
+      <c r="A75" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="B75" s="23" t="n">
+      <c r="B75" s="28" t="n">
         <v>69</v>
       </c>
-      <c r="C75" s="23" t="n">
+      <c r="C75" s="28" t="n">
         <v>30</v>
       </c>
-      <c r="D75" s="23" t="n">
+      <c r="D75" s="28" t="n">
         <v>8</v>
       </c>
-      <c r="E75" s="23" t="n">
+      <c r="E75" s="28" t="n">
         <v>6</v>
       </c>
-      <c r="F75" s="23" t="s">
+      <c r="F75" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="G75" s="24"/>
-      <c r="H75" s="23" t="s">
+      <c r="G75" s="30"/>
+      <c r="H75" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="I75" s="23" t="s">
+      <c r="I75" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="J75" s="23" t="s">
+      <c r="J75" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="23" t="s">
+      <c r="A76" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="B76" s="23" t="n">
+      <c r="B76" s="28" t="n">
         <v>70</v>
       </c>
-      <c r="C76" s="23" t="n">
+      <c r="C76" s="28" t="n">
         <v>29</v>
       </c>
-      <c r="D76" s="23" t="n">
+      <c r="D76" s="28" t="n">
         <v>9</v>
       </c>
-      <c r="E76" s="23" t="n">
+      <c r="E76" s="28" t="n">
         <v>5</v>
       </c>
-      <c r="F76" s="23" t="s">
+      <c r="F76" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="G76" s="24"/>
-      <c r="H76" s="23" t="s">
+      <c r="G76" s="30"/>
+      <c r="H76" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="I76" s="23" t="s">
+      <c r="I76" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="J76" s="23" t="s">
+      <c r="J76" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="23" t="s">
+      <c r="A77" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="B77" s="23" t="n">
+      <c r="B77" s="28" t="n">
         <v>72</v>
       </c>
-      <c r="C77" s="23" t="n">
+      <c r="C77" s="28" t="n">
         <v>28</v>
       </c>
-      <c r="D77" s="23" t="n">
+      <c r="D77" s="28" t="n">
         <v>10</v>
       </c>
-      <c r="E77" s="23" t="n">
+      <c r="E77" s="28" t="n">
         <v>4</v>
       </c>
-      <c r="F77" s="23" t="s">
+      <c r="F77" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="G77" s="24"/>
-      <c r="H77" s="23" t="s">
+      <c r="G77" s="30"/>
+      <c r="H77" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="I77" s="23" t="s">
+      <c r="I77" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="J77" s="23" t="s">
+      <c r="J77" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="23" t="s">
+      <c r="A78" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="B78" s="23" t="n">
+      <c r="B78" s="28" t="n">
         <v>73</v>
       </c>
-      <c r="C78" s="23" t="n">
+      <c r="C78" s="28" t="n">
         <v>26</v>
       </c>
-      <c r="D78" s="23" t="n">
+      <c r="D78" s="28" t="n">
         <v>11</v>
       </c>
-      <c r="E78" s="23" t="n">
+      <c r="E78" s="28" t="n">
         <v>3</v>
       </c>
-      <c r="F78" s="23" t="s">
+      <c r="F78" s="29" t="s">
         <v>76</v>
       </c>
-      <c r="G78" s="24"/>
-      <c r="H78" s="23" t="s">
+      <c r="G78" s="30"/>
+      <c r="H78" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="I78" s="23" t="s">
+      <c r="I78" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="J78" s="23" t="s">
+      <c r="J78" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="23" t="s">
+      <c r="A79" s="28" t="s">
         <v>49</v>
       </c>
-      <c r="B79" s="23" t="n">
+      <c r="B79" s="28" t="n">
         <v>74</v>
       </c>
-      <c r="C79" s="23" t="n">
+      <c r="C79" s="28" t="n">
         <v>25</v>
       </c>
-      <c r="D79" s="23" t="n">
+      <c r="D79" s="28" t="n">
         <v>12</v>
       </c>
-      <c r="E79" s="23" t="n">
+      <c r="E79" s="28" t="n">
         <v>2</v>
       </c>
-      <c r="F79" s="23" t="s">
+      <c r="F79" s="29" t="s">
         <v>77</v>
       </c>
-      <c r="G79" s="24"/>
-      <c r="H79" s="23" t="s">
+      <c r="G79" s="30"/>
+      <c r="H79" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="I79" s="23" t="s">
+      <c r="I79" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="J79" s="23" t="s">
+      <c r="J79" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="23" t="s">
+      <c r="A80" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B80" s="23" t="n">
+      <c r="B80" s="28" t="n">
         <v>81</v>
       </c>
-      <c r="C80" s="23" t="n">
+      <c r="C80" s="28" t="n">
         <v>16</v>
       </c>
-      <c r="D80" s="23" t="n">
+      <c r="D80" s="28" t="n">
         <v>13</v>
       </c>
-      <c r="E80" s="23" t="n">
+      <c r="E80" s="28" t="n">
         <v>1</v>
       </c>
-      <c r="F80" s="23" t="s">
+      <c r="F80" s="29" t="s">
         <v>78</v>
       </c>
-      <c r="G80" s="24"/>
-      <c r="H80" s="23" t="s">
+      <c r="G80" s="30"/>
+      <c r="H80" s="28" t="s">
         <v>65</v>
       </c>
-      <c r="I80" s="23" t="s">
+      <c r="I80" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="J80" s="23" t="s">
+      <c r="J80" s="28" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A81" s="6"/>
-      <c r="B81" s="6"/>
-      <c r="C81" s="6"/>
-      <c r="D81" s="6"/>
-      <c r="E81" s="6"/>
-      <c r="F81" s="6"/>
-      <c r="G81" s="25"/>
-      <c r="H81" s="6"/>
-      <c r="I81" s="6"/>
-      <c r="J81" s="6"/>
-    </row>
+      <c r="A81" s="31" t="s">
+        <v>24</v>
+      </c>
+      <c r="B81" s="31" t="n">
+        <v>28</v>
+      </c>
+      <c r="C81" s="31" t="n">
+        <v>22</v>
+      </c>
+      <c r="D81" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="E81" s="31" t="n">
+        <v>9</v>
+      </c>
+      <c r="F81" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G81" s="33" t="s">
+        <v>80</v>
+      </c>
+      <c r="H81" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="I81" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="J81" s="31" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="82" s="34" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="31" t="s">
+        <v>26</v>
+      </c>
+      <c r="B82" s="31" t="n">
+        <v>31</v>
+      </c>
+      <c r="C82" s="31" t="n">
+        <v>18</v>
+      </c>
+      <c r="D82" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="E82" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="F82" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G82" s="33" t="s">
+        <v>83</v>
+      </c>
+      <c r="H82" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="I82" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="J82" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="K82" s="1"/>
+    </row>
+    <row r="83" s="34" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="31" t="s">
+        <v>10</v>
+      </c>
+      <c r="B83" s="31" t="n">
+        <v>33</v>
+      </c>
+      <c r="C83" s="31" t="n">
+        <v>17</v>
+      </c>
+      <c r="D83" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="E83" s="31" t="n">
+        <v>7</v>
+      </c>
+      <c r="F83" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G83" s="33"/>
+      <c r="H83" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="I83" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="J83" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="K83" s="1"/>
+    </row>
+    <row r="84" s="34" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B84" s="31" t="n">
+        <v>32</v>
+      </c>
+      <c r="C84" s="31" t="n">
+        <v>17</v>
+      </c>
+      <c r="D84" s="31" t="n">
+        <v>4</v>
+      </c>
+      <c r="E84" s="31" t="n">
+        <v>6</v>
+      </c>
+      <c r="F84" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G84" s="33"/>
+      <c r="H84" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="I84" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="J84" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="K84" s="1"/>
+    </row>
+    <row r="85" s="34" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="B85" s="31" t="n">
+        <v>33</v>
+      </c>
+      <c r="C85" s="31" t="n">
+        <v>17</v>
+      </c>
+      <c r="D85" s="31" t="n">
+        <v>5</v>
+      </c>
+      <c r="E85" s="31" t="n">
+        <v>5</v>
+      </c>
+      <c r="F85" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G85" s="33"/>
+      <c r="H85" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="I85" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="J85" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="K85" s="1"/>
+    </row>
+    <row r="86" s="34" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="31" t="s">
+        <v>22</v>
+      </c>
+      <c r="B86" s="31" t="n">
+        <v>33</v>
+      </c>
+      <c r="C86" s="31" t="n">
+        <v>16</v>
+      </c>
+      <c r="D86" s="31" t="n">
+        <v>6</v>
+      </c>
+      <c r="E86" s="31" t="n">
+        <v>4</v>
+      </c>
+      <c r="F86" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G86" s="33"/>
+      <c r="H86" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="I86" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="J86" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="K86" s="1"/>
+    </row>
+    <row r="87" s="34" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="B87" s="31" t="n">
+        <v>34</v>
+      </c>
+      <c r="C87" s="31" t="n">
+        <v>16</v>
+      </c>
+      <c r="D87" s="31" t="n">
+        <v>7</v>
+      </c>
+      <c r="E87" s="31" t="n">
+        <v>3</v>
+      </c>
+      <c r="F87" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G87" s="33"/>
+      <c r="H87" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="I87" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="J87" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="K87" s="1"/>
+    </row>
+    <row r="88" s="34" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="31" t="s">
+        <v>35</v>
+      </c>
+      <c r="B88" s="31" t="n">
+        <v>35</v>
+      </c>
+      <c r="C88" s="31" t="n">
+        <v>15</v>
+      </c>
+      <c r="D88" s="31" t="n">
+        <v>8</v>
+      </c>
+      <c r="E88" s="31" t="n">
+        <v>2</v>
+      </c>
+      <c r="F88" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G88" s="33"/>
+      <c r="H88" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="I88" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="J88" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="K88" s="1"/>
+    </row>
+    <row r="89" s="34" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="31" t="s">
+        <v>39</v>
+      </c>
+      <c r="B89" s="31" t="n">
+        <v>39</v>
+      </c>
+      <c r="C89" s="31" t="n">
+        <v>11</v>
+      </c>
+      <c r="D89" s="31" t="n">
+        <v>9</v>
+      </c>
+      <c r="E89" s="31" t="n">
+        <v>1</v>
+      </c>
+      <c r="F89" s="32" t="s">
+        <v>79</v>
+      </c>
+      <c r="G89" s="33"/>
+      <c r="H89" s="31" t="s">
+        <v>81</v>
+      </c>
+      <c r="I89" s="32" t="s">
+        <v>82</v>
+      </c>
+      <c r="J89" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="K89" s="1"/>
+    </row>
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="34"/>
+      <c r="B90" s="34"/>
+      <c r="C90" s="34"/>
+      <c r="D90" s="34"/>
+      <c r="E90" s="34"/>
+      <c r="F90" s="34"/>
+      <c r="G90" s="34"/>
+      <c r="H90" s="34"/>
+      <c r="I90" s="34"/>
+      <c r="J90" s="34"/>
+    </row>
+    <row r="91" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="34"/>
+      <c r="B91" s="34"/>
+      <c r="C91" s="34"/>
+      <c r="D91" s="34"/>
+      <c r="E91" s="34"/>
+      <c r="F91" s="34"/>
+      <c r="G91" s="34"/>
+      <c r="H91" s="34"/>
+      <c r="I91" s="34"/>
+      <c r="J91" s="34"/>
+    </row>
+    <row r="92" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="34"/>
+      <c r="B92" s="34"/>
+      <c r="C92" s="34"/>
+      <c r="D92" s="34"/>
+      <c r="E92" s="34"/>
+      <c r="F92" s="34"/>
+      <c r="G92" s="34"/>
+      <c r="H92" s="34"/>
+      <c r="I92" s="34"/>
+      <c r="J92" s="34"/>
+    </row>
+    <row r="93" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="34"/>
+      <c r="B93" s="34"/>
+      <c r="C93" s="34"/>
+      <c r="D93" s="34"/>
+      <c r="E93" s="34"/>
+      <c r="F93" s="34"/>
+      <c r="G93" s="34"/>
+      <c r="H93" s="34"/>
+      <c r="I93" s="34"/>
+      <c r="J93" s="34"/>
+    </row>
+    <row r="94" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="34"/>
+      <c r="B94" s="34"/>
+      <c r="C94" s="34"/>
+      <c r="D94" s="34"/>
+      <c r="E94" s="34"/>
+      <c r="F94" s="34"/>
+      <c r="G94" s="34"/>
+      <c r="H94" s="34"/>
+      <c r="I94" s="34"/>
+      <c r="J94" s="34"/>
+    </row>
+    <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="34"/>
+      <c r="B95" s="34"/>
+      <c r="C95" s="34"/>
+      <c r="D95" s="34"/>
+      <c r="E95" s="34"/>
+      <c r="F95" s="34"/>
+      <c r="G95" s="34"/>
+      <c r="H95" s="34"/>
+      <c r="I95" s="34"/>
+      <c r="J95" s="34"/>
+    </row>
+    <row r="96" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="34"/>
+      <c r="B96" s="34"/>
+      <c r="C96" s="34"/>
+      <c r="D96" s="34"/>
+      <c r="E96" s="34"/>
+      <c r="F96" s="34"/>
+      <c r="G96" s="34"/>
+      <c r="H96" s="34"/>
+      <c r="I96" s="34"/>
+      <c r="J96" s="34"/>
+    </row>
+    <row r="97" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="34"/>
+      <c r="B97" s="34"/>
+      <c r="C97" s="34"/>
+      <c r="D97" s="34"/>
+      <c r="E97" s="34"/>
+      <c r="F97" s="34"/>
+      <c r="G97" s="34"/>
+      <c r="H97" s="34"/>
+      <c r="I97" s="34"/>
+      <c r="J97" s="34"/>
+    </row>
+    <row r="98" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="34"/>
+      <c r="B98" s="34"/>
+      <c r="C98" s="34"/>
+      <c r="D98" s="34"/>
+      <c r="E98" s="34"/>
+      <c r="F98" s="34"/>
+      <c r="G98" s="34"/>
+      <c r="H98" s="34"/>
+      <c r="I98" s="34"/>
+      <c r="J98" s="34"/>
+    </row>
+    <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="34"/>
+      <c r="B99" s="34"/>
+      <c r="C99" s="34"/>
+      <c r="D99" s="34"/>
+      <c r="E99" s="34"/>
+      <c r="F99" s="34"/>
+      <c r="G99" s="34"/>
+      <c r="H99" s="34"/>
+      <c r="I99" s="34"/>
+      <c r="J99" s="34"/>
+    </row>
+    <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="34"/>
+      <c r="B100" s="34"/>
+      <c r="C100" s="34"/>
+      <c r="D100" s="34"/>
+      <c r="E100" s="34"/>
+      <c r="F100" s="34"/>
+      <c r="G100" s="34"/>
+      <c r="H100" s="34"/>
+      <c r="I100" s="34"/>
+      <c r="J100" s="34"/>
+    </row>
+    <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="34"/>
+      <c r="B101" s="34"/>
+      <c r="C101" s="34"/>
+      <c r="D101" s="34"/>
+      <c r="E101" s="34"/>
+      <c r="F101" s="34"/>
+      <c r="G101" s="34"/>
+      <c r="H101" s="34"/>
+      <c r="I101" s="34"/>
+      <c r="J101" s="34"/>
+    </row>
+    <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="34"/>
+      <c r="B102" s="34"/>
+      <c r="C102" s="34"/>
+      <c r="D102" s="34"/>
+      <c r="E102" s="34"/>
+      <c r="F102" s="34"/>
+      <c r="G102" s="34"/>
+      <c r="H102" s="34"/>
+      <c r="I102" s="34"/>
+      <c r="J102" s="34"/>
+    </row>
+    <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="34"/>
+      <c r="B103" s="34"/>
+      <c r="C103" s="34"/>
+      <c r="D103" s="34"/>
+      <c r="E103" s="34"/>
+      <c r="F103" s="34"/>
+      <c r="G103" s="34"/>
+      <c r="H103" s="34"/>
+      <c r="I103" s="34"/>
+      <c r="J103" s="34"/>
+    </row>
+    <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="34"/>
+      <c r="B104" s="34"/>
+      <c r="C104" s="34"/>
+      <c r="D104" s="34"/>
+      <c r="E104" s="34"/>
+      <c r="F104" s="34"/>
+      <c r="G104" s="34"/>
+      <c r="H104" s="34"/>
+      <c r="I104" s="34"/>
+      <c r="J104" s="34"/>
+    </row>
+    <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="34"/>
+      <c r="B105" s="34"/>
+      <c r="C105" s="34"/>
+      <c r="D105" s="34"/>
+      <c r="E105" s="34"/>
+      <c r="F105" s="34"/>
+      <c r="G105" s="34"/>
+      <c r="H105" s="34"/>
+      <c r="I105" s="34"/>
+      <c r="J105" s="34"/>
+    </row>
+    <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="34"/>
+      <c r="B106" s="34"/>
+      <c r="C106" s="34"/>
+      <c r="D106" s="34"/>
+      <c r="E106" s="34"/>
+      <c r="F106" s="34"/>
+      <c r="G106" s="34"/>
+      <c r="H106" s="34"/>
+      <c r="I106" s="34"/>
+      <c r="J106" s="34"/>
+    </row>
+    <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="34"/>
+      <c r="B107" s="34"/>
+      <c r="C107" s="34"/>
+      <c r="D107" s="34"/>
+      <c r="E107" s="34"/>
+      <c r="F107" s="34"/>
+      <c r="G107" s="34"/>
+      <c r="H107" s="34"/>
+      <c r="I107" s="34"/>
+      <c r="J107" s="34"/>
+    </row>
+    <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="34"/>
+      <c r="B108" s="34"/>
+      <c r="C108" s="34"/>
+      <c r="D108" s="34"/>
+      <c r="E108" s="34"/>
+      <c r="F108" s="34"/>
+      <c r="G108" s="34"/>
+      <c r="H108" s="34"/>
+      <c r="I108" s="34"/>
+      <c r="J108" s="34"/>
+    </row>
+    <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="34"/>
+      <c r="B109" s="34"/>
+      <c r="C109" s="34"/>
+      <c r="D109" s="34"/>
+      <c r="E109" s="34"/>
+      <c r="F109" s="34"/>
+      <c r="G109" s="34"/>
+      <c r="H109" s="34"/>
+      <c r="I109" s="34"/>
+      <c r="J109" s="34"/>
+    </row>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.3"/>
@@ -3213,8 +3873,8 @@
   </sheetPr>
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="I89 B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3225,90 +3885,90 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>80</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
+      <c r="A1" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
+      <c r="A2" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="C3" s="7"/>
-      <c r="D3" s="7"/>
-      <c r="E3" s="7"/>
+      <c r="A3" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="B3" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C3" s="8"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
     </row>
     <row r="4" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="7" t="s">
-        <v>85</v>
-      </c>
-      <c r="B4" s="23" t="s">
+      <c r="A4" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B4" s="28" t="s">
         <v>66</v>
       </c>
-      <c r="C4" s="7"/>
-      <c r="D4" s="7"/>
-      <c r="E4" s="7"/>
+      <c r="C4" s="8"/>
+      <c r="D4" s="8"/>
+      <c r="E4" s="8"/>
     </row>
     <row r="5" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="7"/>
-      <c r="B5" s="7"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
+      <c r="A5" s="8"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="7"/>
-      <c r="B6" s="7"/>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="7"/>
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="8"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="7"/>
-      <c r="B8" s="7"/>
-      <c r="C8" s="7"/>
-      <c r="D8" s="7"/>
-      <c r="E8" s="7"/>
+      <c r="A8" s="8"/>
+      <c r="B8" s="8"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8"/>
+      <c r="E8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="7"/>
-      <c r="B9" s="7"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="7"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
     </row>
     <row r="10" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="7"/>
-      <c r="B10" s="7"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="7"/>
-      <c r="E10" s="7"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="8"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
+      <c r="E10" s="8"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3319,4 +3979,468 @@
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J20"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="1" sqref="I89 E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="36"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36" t="n">
+        <v>1</v>
+      </c>
+      <c r="E1" s="36"/>
+      <c r="F1" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="38"/>
+      <c r="H1" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I1" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J1" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="36"/>
+      <c r="B2" s="36"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" s="36"/>
+      <c r="F2" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G2" s="38"/>
+      <c r="H2" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I2" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J2" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="36"/>
+      <c r="B3" s="36"/>
+      <c r="C3" s="36"/>
+      <c r="D3" s="36" t="n">
+        <v>3</v>
+      </c>
+      <c r="E3" s="36"/>
+      <c r="F3" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G3" s="38"/>
+      <c r="H3" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I3" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J3" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="36"/>
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36" t="n">
+        <v>4</v>
+      </c>
+      <c r="E4" s="36"/>
+      <c r="F4" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G4" s="38"/>
+      <c r="H4" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I4" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J4" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="36"/>
+      <c r="B5" s="36"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="36" t="n">
+        <v>5</v>
+      </c>
+      <c r="E5" s="36"/>
+      <c r="F5" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G5" s="38"/>
+      <c r="H5" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I5" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J5" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="36"/>
+      <c r="B6" s="36"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="36" t="n">
+        <v>6</v>
+      </c>
+      <c r="E6" s="36"/>
+      <c r="F6" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G6" s="38"/>
+      <c r="H6" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J6" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="36"/>
+      <c r="B7" s="36"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="36" t="n">
+        <v>7</v>
+      </c>
+      <c r="E7" s="36"/>
+      <c r="F7" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G7" s="38"/>
+      <c r="H7" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I7" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J7" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="36"/>
+      <c r="B8" s="36"/>
+      <c r="C8" s="36"/>
+      <c r="D8" s="36" t="n">
+        <v>8</v>
+      </c>
+      <c r="E8" s="36"/>
+      <c r="F8" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G8" s="38"/>
+      <c r="H8" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I8" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J8" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="36"/>
+      <c r="B9" s="36"/>
+      <c r="C9" s="36"/>
+      <c r="D9" s="36" t="n">
+        <v>9</v>
+      </c>
+      <c r="E9" s="36"/>
+      <c r="F9" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G9" s="38"/>
+      <c r="H9" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I9" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J9" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="36"/>
+      <c r="B10" s="36"/>
+      <c r="C10" s="36"/>
+      <c r="D10" s="36" t="n">
+        <v>10</v>
+      </c>
+      <c r="E10" s="36"/>
+      <c r="F10" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G10" s="38"/>
+      <c r="H10" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I10" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J10" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="36"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36" t="n">
+        <v>11</v>
+      </c>
+      <c r="E11" s="36"/>
+      <c r="F11" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="38"/>
+      <c r="H11" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J11" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="36"/>
+      <c r="B12" s="36"/>
+      <c r="C12" s="36"/>
+      <c r="D12" s="36" t="n">
+        <v>12</v>
+      </c>
+      <c r="E12" s="36"/>
+      <c r="F12" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G12" s="38"/>
+      <c r="H12" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I12" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J12" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="36"/>
+      <c r="B13" s="36"/>
+      <c r="C13" s="36"/>
+      <c r="D13" s="36" t="n">
+        <v>13</v>
+      </c>
+      <c r="E13" s="36"/>
+      <c r="F13" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G13" s="38"/>
+      <c r="H13" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I13" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J13" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="36"/>
+      <c r="B14" s="36"/>
+      <c r="C14" s="36"/>
+      <c r="D14" s="36" t="n">
+        <v>14</v>
+      </c>
+      <c r="E14" s="36"/>
+      <c r="F14" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G14" s="38"/>
+      <c r="H14" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I14" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J14" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="36"/>
+      <c r="B15" s="36"/>
+      <c r="C15" s="36"/>
+      <c r="D15" s="36" t="n">
+        <v>15</v>
+      </c>
+      <c r="E15" s="36"/>
+      <c r="F15" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G15" s="38"/>
+      <c r="H15" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I15" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J15" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="36"/>
+      <c r="B16" s="36"/>
+      <c r="C16" s="36"/>
+      <c r="D16" s="36" t="n">
+        <v>16</v>
+      </c>
+      <c r="E16" s="36"/>
+      <c r="F16" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="38"/>
+      <c r="H16" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I16" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J16" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="36"/>
+      <c r="B17" s="36"/>
+      <c r="C17" s="36"/>
+      <c r="D17" s="36" t="n">
+        <v>17</v>
+      </c>
+      <c r="E17" s="36"/>
+      <c r="F17" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G17" s="38"/>
+      <c r="H17" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I17" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J17" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="36"/>
+      <c r="B18" s="36"/>
+      <c r="C18" s="36"/>
+      <c r="D18" s="36" t="n">
+        <v>18</v>
+      </c>
+      <c r="E18" s="36"/>
+      <c r="F18" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G18" s="38"/>
+      <c r="H18" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I18" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J18" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="36"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36" t="n">
+        <v>19</v>
+      </c>
+      <c r="E19" s="36"/>
+      <c r="F19" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" s="38"/>
+      <c r="H19" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I19" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J19" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="36"/>
+      <c r="B20" s="36"/>
+      <c r="C20" s="36"/>
+      <c r="D20" s="36" t="n">
+        <v>20</v>
+      </c>
+      <c r="E20" s="36"/>
+      <c r="F20" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="G20" s="38"/>
+      <c r="H20" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="I20" s="37" t="s">
+        <v>91</v>
+      </c>
+      <c r="J20" s="36" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>